<commit_message>
Temporary bolding for edit in progress.
</commit_message>
<xml_diff>
--- a/edited_data.xlsx
+++ b/edited_data.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BD$368</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AT$369</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3250" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3255" uniqueCount="503">
   <si>
     <t>Adachi, P. J. C., &amp; Willoughby, T. (2011). S1</t>
   </si>
@@ -1196,9 +1196,6 @@
     <t>Total state hostility</t>
   </si>
   <si>
-    <t>Sestir, M. A., &amp; Bartholow, B. D. (2010).</t>
-  </si>
-  <si>
     <t>aggressive behaviour (0 min delay)</t>
   </si>
   <si>
@@ -1527,13 +1524,25 @@
   </si>
   <si>
     <t>verbal aggression subscale</t>
+  </si>
+  <si>
+    <t>Sestir, M. A., &amp; Bartholow, B. D. (2010). S2</t>
+  </si>
+  <si>
+    <t>Sestir, M. A., &amp; Bartholow, B. D. (2010). S1</t>
+  </si>
+  <si>
+    <t>word and story completion</t>
+  </si>
+  <si>
+    <t>Sestir, M. A., &amp; Bartholow, B. D. (2010). S3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1541,13 +1550,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1559,15 +1580,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1846,192 +1870,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD367"/>
+  <dimension ref="A1:BD368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AT177" sqref="AT177"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF224" sqref="AF224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
-    <col min="7" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="9" max="33" width="19.42578125" hidden="1" customWidth="1"/>
-    <col min="34" max="36" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="31" width="19.42578125" hidden="1" customWidth="1"/>
+    <col min="32" max="33" width="19.42578125" customWidth="1"/>
+    <col min="34" max="36" width="9.140625" customWidth="1"/>
     <col min="40" max="40" width="12" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="85.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B1" t="s">
         <v>432</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>433</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>434</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>435</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>436</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>448</v>
+      </c>
+      <c r="H1" t="s">
+        <v>449</v>
+      </c>
+      <c r="I1" t="s">
+        <v>450</v>
+      </c>
+      <c r="J1" t="s">
+        <v>451</v>
+      </c>
+      <c r="K1" t="s">
+        <v>452</v>
+      </c>
+      <c r="L1" t="s">
+        <v>453</v>
+      </c>
+      <c r="M1" t="s">
+        <v>454</v>
+      </c>
+      <c r="N1" t="s">
+        <v>455</v>
+      </c>
+      <c r="O1" t="s">
+        <v>456</v>
+      </c>
+      <c r="P1" t="s">
+        <v>460</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>457</v>
+      </c>
+      <c r="R1" t="s">
+        <v>458</v>
+      </c>
+      <c r="S1" t="s">
+        <v>459</v>
+      </c>
+      <c r="T1" t="s">
+        <v>461</v>
+      </c>
+      <c r="U1" t="s">
+        <v>462</v>
+      </c>
+      <c r="V1" t="s">
+        <v>463</v>
+      </c>
+      <c r="W1" t="s">
+        <v>464</v>
+      </c>
+      <c r="X1" t="s">
+        <v>465</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>466</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>467</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>468</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>469</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>470</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>471</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>472</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>473</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>474</v>
+      </c>
+      <c r="AH1" t="s">
         <v>437</v>
       </c>
-      <c r="G1" t="s">
-        <v>449</v>
-      </c>
-      <c r="H1" t="s">
-        <v>450</v>
-      </c>
-      <c r="I1" t="s">
-        <v>451</v>
-      </c>
-      <c r="J1" t="s">
-        <v>452</v>
-      </c>
-      <c r="K1" t="s">
-        <v>453</v>
-      </c>
-      <c r="L1" t="s">
-        <v>454</v>
-      </c>
-      <c r="M1" t="s">
-        <v>455</v>
-      </c>
-      <c r="N1" t="s">
-        <v>456</v>
-      </c>
-      <c r="O1" t="s">
-        <v>457</v>
-      </c>
-      <c r="P1" t="s">
-        <v>461</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>458</v>
-      </c>
-      <c r="R1" t="s">
-        <v>459</v>
-      </c>
-      <c r="S1" t="s">
-        <v>460</v>
-      </c>
-      <c r="T1" t="s">
-        <v>462</v>
-      </c>
-      <c r="U1" t="s">
-        <v>463</v>
-      </c>
-      <c r="V1" t="s">
-        <v>464</v>
-      </c>
-      <c r="W1" t="s">
-        <v>465</v>
-      </c>
-      <c r="X1" t="s">
-        <v>466</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>467</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>468</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>469</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>470</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>471</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>472</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>473</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>474</v>
-      </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>475</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
+        <v>476</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>446</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>447</v>
+      </c>
+      <c r="AM1" t="s">
         <v>438</v>
       </c>
-      <c r="AI1" t="s">
-        <v>476</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="AN1" t="s">
+        <v>439</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>440</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>441</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>442</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>443</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>444</v>
+      </c>
+      <c r="AT1" t="s">
         <v>477</v>
       </c>
-      <c r="AK1" t="s">
-        <v>447</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>448</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>439</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>440</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>441</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>442</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>443</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>444</v>
-      </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>486</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>487</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>488</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>481</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>482</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>483</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>484</v>
+      </c>
+      <c r="BC1" t="s">
         <v>445</v>
       </c>
-      <c r="AT1" t="s">
-        <v>478</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>486</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>487</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>488</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>489</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>482</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>483</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>484</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>485</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>446</v>
-      </c>
       <c r="BD1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
@@ -2512,7 +2538,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J9">
         <f>AVERAGE(0.44, 0.5)</f>
@@ -2561,10 +2587,10 @@
         <v>9</v>
       </c>
       <c r="AU9" t="s">
+        <v>489</v>
+      </c>
+      <c r="AV9" t="s">
         <v>490</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>491</v>
       </c>
       <c r="AY9">
         <v>0.5</v>
@@ -2573,7 +2599,7 @@
         <v>0.44</v>
       </c>
       <c r="BC9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="BD9" t="s">
         <v>22</v>
@@ -2933,7 +2959,7 @@
         <v>87</v>
       </c>
       <c r="U15" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK15">
         <v>0.11775505103579501</v>
@@ -3007,7 +3033,7 @@
         <v>87</v>
       </c>
       <c r="U16" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK16" s="1">
         <v>1.88132384358922E-2</v>
@@ -3081,7 +3107,7 @@
         <v>87</v>
       </c>
       <c r="U17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK17">
         <v>0.105854786920116</v>
@@ -3155,7 +3181,7 @@
         <v>23</v>
       </c>
       <c r="U18" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK18">
         <v>0.38708835994406798</v>
@@ -3229,7 +3255,7 @@
         <v>23</v>
       </c>
       <c r="U19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK19">
         <v>0.37324680142328898</v>
@@ -3303,7 +3329,7 @@
         <v>22</v>
       </c>
       <c r="U20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK20">
         <v>0.29530730609491901</v>
@@ -3377,7 +3403,7 @@
         <v>23</v>
       </c>
       <c r="U21" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK21">
         <v>0.157908384915591</v>
@@ -3782,7 +3808,7 @@
         <v>18</v>
       </c>
       <c r="U27" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK27">
         <v>-0.32001329437029802</v>
@@ -3859,7 +3885,7 @@
         <v>18</v>
       </c>
       <c r="U28" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK28">
         <v>0.368305806793924</v>
@@ -4001,7 +4027,7 @@
         <v>41</v>
       </c>
       <c r="U30" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK30" s="1">
         <v>6.5745978697184806E-2</v>
@@ -4075,7 +4101,7 @@
         <v>41</v>
       </c>
       <c r="U31" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK31" s="1">
         <v>1.47224692839925E-2</v>
@@ -4459,7 +4485,7 @@
         <v>18</v>
       </c>
       <c r="U37" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK37">
         <v>0.23238050000631399</v>
@@ -4533,7 +4559,7 @@
         <v>18</v>
       </c>
       <c r="U38" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK38">
         <v>-0.16973737763046201</v>
@@ -4805,7 +4831,7 @@
         <v>29</v>
       </c>
       <c r="U42" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK42">
         <v>-0.191538071371774</v>
@@ -4879,7 +4905,7 @@
         <v>29</v>
       </c>
       <c r="U43" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK43">
         <v>0.14730956928116101</v>
@@ -4953,7 +4979,7 @@
         <v>29</v>
       </c>
       <c r="U44" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK44" s="1">
         <v>-1.00046436056182E-2</v>
@@ -6468,7 +6494,7 @@
         <v>25</v>
       </c>
       <c r="U68" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AK68">
         <v>3.5154698054722003E-2</v>
@@ -6542,7 +6568,7 @@
         <v>26</v>
       </c>
       <c r="U69" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AK69">
         <v>-0.11588005146689299</v>
@@ -6616,7 +6642,7 @@
         <v>25</v>
       </c>
       <c r="U70" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AK70" s="1">
         <v>3.1836903298351697E-2</v>
@@ -6690,7 +6716,7 @@
         <v>26</v>
       </c>
       <c r="U71" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AK71">
         <v>-0.11565463171158399</v>
@@ -6956,7 +6982,7 @@
         <v>13</v>
       </c>
       <c r="U75" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK75">
         <v>0.43481823629979299</v>
@@ -7160,7 +7186,7 @@
         <v>37</v>
       </c>
       <c r="U78" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK78">
         <v>0.30197010641017102</v>
@@ -8064,7 +8090,7 @@
         <v>169</v>
       </c>
       <c r="U92" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK92">
         <v>0.14788611324801701</v>
@@ -10093,7 +10119,7 @@
         <v>38</v>
       </c>
       <c r="U124" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK124">
         <v>0.20307294859175301</v>
@@ -10167,7 +10193,7 @@
         <v>21</v>
       </c>
       <c r="U125" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK125">
         <v>0.359136094885042</v>
@@ -10365,7 +10391,7 @@
         <v>20</v>
       </c>
       <c r="U128" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK128" s="1">
         <v>-1.22028373675277E-2</v>
@@ -10439,7 +10465,7 @@
         <v>20</v>
       </c>
       <c r="U129" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK129">
         <v>0.45471427033982198</v>
@@ -10513,7 +10539,7 @@
         <v>20</v>
       </c>
       <c r="U130" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK130">
         <v>0.73201968270769102</v>
@@ -10587,7 +10613,7 @@
         <v>20</v>
       </c>
       <c r="U131" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK131">
         <v>0.63694371197226296</v>
@@ -10998,7 +11024,7 @@
         <v>8</v>
       </c>
       <c r="U137" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK137">
         <v>0.40584569331961901</v>
@@ -11332,7 +11358,7 @@
         <v>42</v>
       </c>
       <c r="U142" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK142">
         <v>0.22443290236982399</v>
@@ -11666,7 +11692,7 @@
         <v>57</v>
       </c>
       <c r="U147" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK147">
         <v>0.15768945703450199</v>
@@ -11802,7 +11828,7 @@
         <v>9</v>
       </c>
       <c r="U149" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK149" s="1">
         <v>9.78372160424551E-2</v>
@@ -11876,7 +11902,7 @@
         <v>34</v>
       </c>
       <c r="U150" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK150">
         <v>-2.6005845470728001E-2</v>
@@ -11950,7 +11976,7 @@
         <v>34</v>
       </c>
       <c r="U151" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK151">
         <v>0.18219642438814199</v>
@@ -12024,7 +12050,7 @@
         <v>34</v>
       </c>
       <c r="U152" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK152" s="1">
         <v>-8.1130243527845203E-2</v>
@@ -13515,13 +13541,13 @@
         <v>2</v>
       </c>
       <c r="D176" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E176" t="s">
         <v>1</v>
       </c>
       <c r="F176" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AF176">
         <v>153</v>
@@ -13554,7 +13580,7 @@
         <v>3</v>
       </c>
       <c r="BC176" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="BD176" t="s">
         <v>310</v>
@@ -13571,13 +13597,13 @@
         <v>2</v>
       </c>
       <c r="D177" t="s">
+        <v>493</v>
+      </c>
+      <c r="E177" t="s">
+        <v>1</v>
+      </c>
+      <c r="F177" t="s">
         <v>494</v>
-      </c>
-      <c r="E177" t="s">
-        <v>1</v>
-      </c>
-      <c r="F177" t="s">
-        <v>495</v>
       </c>
       <c r="AF177">
         <v>153</v>
@@ -13610,13 +13636,13 @@
         <v>3</v>
       </c>
       <c r="AU177" t="s">
+        <v>497</v>
+      </c>
+      <c r="AV177" t="s">
         <v>498</v>
       </c>
-      <c r="AV177" t="s">
-        <v>499</v>
-      </c>
       <c r="BC177" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="BD177" t="s">
         <v>310</v>
@@ -13639,7 +13665,7 @@
         <v>1</v>
       </c>
       <c r="F178" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AF178">
         <v>153</v>
@@ -13672,7 +13698,7 @@
         <v>3</v>
       </c>
       <c r="BC178" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="BD178" t="s">
         <v>310</v>
@@ -13920,7 +13946,7 @@
         <v>26</v>
       </c>
       <c r="U182" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK182">
         <v>0.204869051416882</v>
@@ -13994,7 +14020,7 @@
         <v>26</v>
       </c>
       <c r="U183" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK183">
         <v>0.48413896698103398</v>
@@ -14068,7 +14094,7 @@
         <v>26</v>
       </c>
       <c r="U184" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK184">
         <v>0.177114366993189</v>
@@ -14142,7 +14168,7 @@
         <v>26</v>
       </c>
       <c r="U185" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK185">
         <v>0.39554761159184498</v>
@@ -14216,7 +14242,7 @@
         <v>26</v>
       </c>
       <c r="U186" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK186">
         <v>0.165623109821497</v>
@@ -14290,7 +14316,7 @@
         <v>26</v>
       </c>
       <c r="U187" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK187">
         <v>0.38899447096877698</v>
@@ -14426,7 +14452,7 @@
         <v>542</v>
       </c>
       <c r="U189" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK189">
         <v>0.13385924414716799</v>
@@ -14500,7 +14526,7 @@
         <v>540</v>
       </c>
       <c r="U190" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK190">
         <v>0.18823993670091901</v>
@@ -15814,7 +15840,7 @@
         <v>59</v>
       </c>
       <c r="U211" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK211" s="1">
         <v>5.1455950994510703E-2</v>
@@ -16674,7 +16700,7 @@
         <v>84</v>
       </c>
       <c r="U224" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK224">
         <v>0.43045215970323403</v>
@@ -16748,7 +16774,7 @@
         <v>84</v>
       </c>
       <c r="U225" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK225">
         <v>0.241289668231458</v>
@@ -17329,39 +17355,64 @@
       </c>
     </row>
     <row r="234" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
+      <c r="A234" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D234" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="B234" t="s">
-        <v>1</v>
-      </c>
-      <c r="C234" t="s">
-        <v>2</v>
-      </c>
-      <c r="D234" t="s">
-        <v>390</v>
-      </c>
-      <c r="E234" t="s">
-        <v>1</v>
-      </c>
-      <c r="F234" t="s">
+      <c r="E234" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F234" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J234">
+      <c r="G234" s="3"/>
+      <c r="H234" s="3"/>
+      <c r="I234" s="3"/>
+      <c r="J234" s="3">
         <v>0.4</v>
       </c>
-      <c r="K234">
+      <c r="K234" s="3">
         <v>1.0488432000000001E-2</v>
       </c>
-      <c r="L234">
+      <c r="L234" s="3">
         <v>91</v>
       </c>
-      <c r="M234">
+      <c r="M234" s="3">
         <v>90</v>
       </c>
-      <c r="N234">
-        <v>3</v>
-      </c>
+      <c r="N234" s="3">
+        <v>3</v>
+      </c>
+      <c r="O234" s="3"/>
+      <c r="P234" s="3"/>
+      <c r="Q234" s="3"/>
+      <c r="R234" s="3"/>
+      <c r="S234" s="3"/>
+      <c r="T234" s="3"/>
+      <c r="U234" s="3"/>
+      <c r="V234" s="3"/>
+      <c r="W234" s="3"/>
+      <c r="X234" s="3"/>
+      <c r="Y234" s="3"/>
+      <c r="Z234" s="3"/>
+      <c r="AA234" s="3"/>
+      <c r="AB234" s="3"/>
+      <c r="AC234" s="3"/>
+      <c r="AD234" s="3"/>
+      <c r="AE234" s="3"/>
+      <c r="AF234" s="3"/>
+      <c r="AG234" s="3"/>
+      <c r="AH234" s="3"/>
+      <c r="AI234" s="3"/>
+      <c r="AJ234" s="3"/>
       <c r="AK234">
         <v>0.196113257100091</v>
       </c>
@@ -17393,37 +17444,64 @@
         <v>9</v>
       </c>
       <c r="BD234" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="235" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>389</v>
-      </c>
-      <c r="B235" t="s">
-        <v>1</v>
-      </c>
-      <c r="C235" t="s">
-        <v>2</v>
-      </c>
-      <c r="D235" t="s">
+      <c r="A235" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D235" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="E235" t="s">
-        <v>1</v>
-      </c>
-      <c r="F235" t="s">
+      <c r="E235" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F235" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G235">
+      <c r="G235" s="3">
         <v>0.11</v>
       </c>
-      <c r="H235">
+      <c r="H235" s="3">
         <v>181</v>
       </c>
-      <c r="I235">
-        <v>3</v>
-      </c>
+      <c r="I235" s="3">
+        <v>3</v>
+      </c>
+      <c r="J235" s="3"/>
+      <c r="K235" s="3"/>
+      <c r="L235" s="3"/>
+      <c r="M235" s="3"/>
+      <c r="N235" s="3"/>
+      <c r="O235" s="3"/>
+      <c r="P235" s="3"/>
+      <c r="Q235" s="3"/>
+      <c r="R235" s="3"/>
+      <c r="S235" s="3"/>
+      <c r="T235" s="3"/>
+      <c r="U235" s="3"/>
+      <c r="V235" s="3"/>
+      <c r="W235" s="3"/>
+      <c r="X235" s="3"/>
+      <c r="Y235" s="3"/>
+      <c r="Z235" s="3"/>
+      <c r="AA235" s="3"/>
+      <c r="AB235" s="3"/>
+      <c r="AC235" s="3"/>
+      <c r="AD235" s="3"/>
+      <c r="AE235" s="3"/>
+      <c r="AF235" s="3"/>
+      <c r="AG235" s="3"/>
+      <c r="AH235" s="3"/>
+      <c r="AI235" s="3"/>
+      <c r="AJ235" s="3"/>
       <c r="AK235">
         <v>0.11</v>
       </c>
@@ -17455,37 +17533,64 @@
         <v>9</v>
       </c>
       <c r="BD235" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="236" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A236" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D236" s="3" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="236" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>389</v>
-      </c>
-      <c r="B236" t="s">
-        <v>1</v>
-      </c>
-      <c r="C236" t="s">
-        <v>2</v>
-      </c>
-      <c r="D236" t="s">
-        <v>393</v>
-      </c>
-      <c r="E236" t="s">
-        <v>1</v>
-      </c>
-      <c r="F236" t="s">
+      <c r="E236" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F236" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G236">
+      <c r="G236" s="3">
         <v>0.21</v>
       </c>
-      <c r="H236">
+      <c r="H236" s="3">
         <v>181</v>
       </c>
-      <c r="I236">
-        <v>3</v>
-      </c>
+      <c r="I236" s="3">
+        <v>3</v>
+      </c>
+      <c r="J236" s="3"/>
+      <c r="K236" s="3"/>
+      <c r="L236" s="3"/>
+      <c r="M236" s="3"/>
+      <c r="N236" s="3"/>
+      <c r="O236" s="3"/>
+      <c r="P236" s="3"/>
+      <c r="Q236" s="3"/>
+      <c r="R236" s="3"/>
+      <c r="S236" s="3"/>
+      <c r="T236" s="3"/>
+      <c r="U236" s="3"/>
+      <c r="V236" s="3"/>
+      <c r="W236" s="3"/>
+      <c r="X236" s="3"/>
+      <c r="Y236" s="3"/>
+      <c r="Z236" s="3"/>
+      <c r="AA236" s="3"/>
+      <c r="AB236" s="3"/>
+      <c r="AC236" s="3"/>
+      <c r="AD236" s="3"/>
+      <c r="AE236" s="3"/>
+      <c r="AF236" s="3"/>
+      <c r="AG236" s="3"/>
+      <c r="AH236" s="3"/>
+      <c r="AI236" s="3"/>
+      <c r="AJ236" s="3"/>
       <c r="AK236">
         <v>0.21</v>
       </c>
@@ -17517,80 +17622,60 @@
         <v>9</v>
       </c>
       <c r="BD236" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="237" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>394</v>
-      </c>
-      <c r="B237" t="s">
-        <v>1</v>
-      </c>
-      <c r="C237" t="s">
-        <v>2</v>
-      </c>
-      <c r="D237" t="s">
-        <v>395</v>
-      </c>
-      <c r="E237" t="s">
-        <v>1</v>
-      </c>
-      <c r="F237" t="s">
-        <v>19</v>
-      </c>
-      <c r="J237">
-        <v>0.2</v>
-      </c>
-      <c r="K237">
-        <v>1.3947421999999999E-2</v>
-      </c>
-      <c r="L237">
-        <v>137</v>
-      </c>
-      <c r="M237">
-        <v>152</v>
-      </c>
-      <c r="N237">
-        <v>3</v>
-      </c>
-      <c r="AK237" s="1">
-        <v>9.9370925693902504E-2</v>
-      </c>
-      <c r="AL237" s="1">
-        <v>5.80987141556355E-2</v>
-      </c>
-      <c r="AM237">
-        <v>9.9699959427935997E-2</v>
-      </c>
-      <c r="AN237" s="1">
-        <v>5.8678136156606199E-2</v>
-      </c>
-      <c r="AO237" t="s">
-        <v>26</v>
-      </c>
-      <c r="AP237" t="s">
-        <v>6</v>
-      </c>
-      <c r="AQ237" t="s">
-        <v>7</v>
-      </c>
-      <c r="AR237" t="s">
-        <v>8</v>
-      </c>
-      <c r="AS237">
-        <v>3</v>
-      </c>
-      <c r="AT237" t="s">
-        <v>116</v>
-      </c>
-      <c r="BD237" t="s">
-        <v>396</v>
-      </c>
+      <c r="A237" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F237" s="3"/>
+      <c r="G237" s="3"/>
+      <c r="H237" s="3"/>
+      <c r="I237" s="3"/>
+      <c r="J237" s="3"/>
+      <c r="K237" s="3"/>
+      <c r="L237" s="3"/>
+      <c r="M237" s="3"/>
+      <c r="N237" s="3"/>
+      <c r="O237" s="3"/>
+      <c r="P237" s="3"/>
+      <c r="Q237" s="3"/>
+      <c r="R237" s="3"/>
+      <c r="S237" s="3"/>
+      <c r="T237" s="3"/>
+      <c r="U237" s="3"/>
+      <c r="V237" s="3"/>
+      <c r="W237" s="3"/>
+      <c r="X237" s="3"/>
+      <c r="Y237" s="3"/>
+      <c r="Z237" s="3"/>
+      <c r="AA237" s="3"/>
+      <c r="AB237" s="3"/>
+      <c r="AC237" s="3"/>
+      <c r="AD237" s="3"/>
+      <c r="AE237" s="3"/>
+      <c r="AF237" s="3"/>
+      <c r="AG237" s="3"/>
+      <c r="AH237" s="3"/>
+      <c r="AI237" s="3"/>
+      <c r="AJ237" s="3"/>
     </row>
     <row r="238" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B238" t="s">
         <v>1</v>
@@ -17599,7 +17684,7 @@
         <v>2</v>
       </c>
       <c r="D238" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E238" t="s">
         <v>1</v>
@@ -17608,34 +17693,34 @@
         <v>19</v>
       </c>
       <c r="J238">
-        <v>0.37</v>
+        <v>0.2</v>
       </c>
       <c r="K238">
-        <v>3.0884330000000002E-2</v>
+        <v>1.3947421999999999E-2</v>
       </c>
       <c r="L238">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="M238">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="N238">
-        <v>1</v>
-      </c>
-      <c r="AK238">
-        <v>0.181731388425629</v>
+        <v>3</v>
+      </c>
+      <c r="AK238" s="1">
+        <v>9.9370925693902504E-2</v>
       </c>
       <c r="AL238" s="1">
-        <v>8.3466456439473397E-2</v>
+        <v>5.80987141556355E-2</v>
       </c>
       <c r="AM238">
-        <v>0.183772630839275</v>
+        <v>9.9699959427935997E-2</v>
       </c>
       <c r="AN238" s="1">
-        <v>8.6317193763445696E-2</v>
+        <v>5.8678136156606199E-2</v>
       </c>
       <c r="AO238" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="AP238" t="s">
         <v>6</v>
@@ -17653,21 +17738,21 @@
         <v>116</v>
       </c>
       <c r="BD238" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="239" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
+        <v>396</v>
+      </c>
+      <c r="B239" t="s">
+        <v>1</v>
+      </c>
+      <c r="C239" t="s">
+        <v>2</v>
+      </c>
+      <c r="D239" t="s">
         <v>397</v>
-      </c>
-      <c r="B239" t="s">
-        <v>1</v>
-      </c>
-      <c r="C239" t="s">
-        <v>2</v>
-      </c>
-      <c r="D239" t="s">
-        <v>245</v>
       </c>
       <c r="E239" t="s">
         <v>1</v>
@@ -17676,10 +17761,10 @@
         <v>19</v>
       </c>
       <c r="J239">
-        <v>-0.05</v>
+        <v>0.37</v>
       </c>
       <c r="K239">
-        <v>3.0375238999999998E-2</v>
+        <v>3.0884330000000002E-2</v>
       </c>
       <c r="L239">
         <v>63</v>
@@ -17688,25 +17773,25 @@
         <v>69</v>
       </c>
       <c r="N239">
-        <v>3</v>
-      </c>
-      <c r="AK239" s="1">
-        <v>2.49663755409265E-2</v>
+        <v>1</v>
+      </c>
+      <c r="AK239">
+        <v>0.181731388425629</v>
       </c>
       <c r="AL239" s="1">
-        <v>8.6971018806489594E-2</v>
-      </c>
-      <c r="AM239" s="1">
-        <v>2.49715648281152E-2</v>
+        <v>8.3466456439473397E-2</v>
+      </c>
+      <c r="AM239">
+        <v>0.183772630839275</v>
       </c>
       <c r="AN239" s="1">
-        <v>8.7025263385626397E-2</v>
+        <v>8.6317193763445696E-2</v>
       </c>
       <c r="AO239" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="AP239" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="AQ239" t="s">
         <v>7</v>
@@ -17721,12 +17806,12 @@
         <v>116</v>
       </c>
       <c r="BD239" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="240" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B240" t="s">
         <v>1</v>
@@ -17735,7 +17820,7 @@
         <v>2</v>
       </c>
       <c r="D240" t="s">
-        <v>400</v>
+        <v>245</v>
       </c>
       <c r="E240" t="s">
         <v>1</v>
@@ -17744,10 +17829,10 @@
         <v>19</v>
       </c>
       <c r="J240">
-        <v>0.37</v>
+        <v>-0.05</v>
       </c>
       <c r="K240">
-        <v>3.0884330000000002E-2</v>
+        <v>3.0375238999999998E-2</v>
       </c>
       <c r="L240">
         <v>63</v>
@@ -17756,25 +17841,25 @@
         <v>69</v>
       </c>
       <c r="N240">
-        <v>1</v>
-      </c>
-      <c r="AK240">
-        <v>0.181731388425629</v>
+        <v>3</v>
+      </c>
+      <c r="AK240" s="1">
+        <v>2.49663755409265E-2</v>
       </c>
       <c r="AL240" s="1">
-        <v>8.3466456439473397E-2</v>
-      </c>
-      <c r="AM240">
-        <v>0.183772630839275</v>
+        <v>8.6971018806489594E-2</v>
+      </c>
+      <c r="AM240" s="1">
+        <v>2.49715648281152E-2</v>
       </c>
       <c r="AN240" s="1">
-        <v>8.6317193763445696E-2</v>
+        <v>8.7025263385626397E-2</v>
       </c>
       <c r="AO240" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="AP240" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="AQ240" t="s">
         <v>7</v>
@@ -17789,57 +17874,63 @@
         <v>116</v>
       </c>
       <c r="BD240" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="241" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B241" t="s">
         <v>1</v>
       </c>
       <c r="C241" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D241" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="E241" t="s">
         <v>1</v>
       </c>
       <c r="F241" t="s">
-        <v>4</v>
-      </c>
-      <c r="G241">
-        <v>0.19</v>
-      </c>
-      <c r="H241">
-        <v>168</v>
-      </c>
-      <c r="I241">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="J241">
+        <v>0.37</v>
+      </c>
+      <c r="K241">
+        <v>3.0884330000000002E-2</v>
+      </c>
+      <c r="L241">
+        <v>63</v>
+      </c>
+      <c r="M241">
+        <v>69</v>
+      </c>
+      <c r="N241">
+        <v>1</v>
       </c>
       <c r="AK241">
-        <v>0.19</v>
+        <v>0.181731388425629</v>
       </c>
       <c r="AL241" s="1">
-        <v>7.5039513227729199E-2</v>
-      </c>
-      <c r="AM241" s="1">
-        <v>0.192337169219545</v>
+        <v>8.3466456439473397E-2</v>
+      </c>
+      <c r="AM241">
+        <v>0.183772630839275</v>
       </c>
       <c r="AN241" s="1">
-        <v>7.7849894416152296E-2</v>
+        <v>8.6317193763445696E-2</v>
       </c>
       <c r="AO241" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="AP241" t="s">
         <v>6</v>
       </c>
       <c r="AQ241" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="AR241" t="s">
         <v>8</v>
@@ -17851,21 +17942,21 @@
         <v>116</v>
       </c>
       <c r="BD241" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="242" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
+        <v>400</v>
+      </c>
+      <c r="B242" t="s">
+        <v>1</v>
+      </c>
+      <c r="C242" t="s">
+        <v>1</v>
+      </c>
+      <c r="D242" t="s">
         <v>401</v>
-      </c>
-      <c r="B242" t="s">
-        <v>1</v>
-      </c>
-      <c r="C242" t="s">
-        <v>1</v>
-      </c>
-      <c r="D242" t="s">
-        <v>293</v>
       </c>
       <c r="E242" t="s">
         <v>1</v>
@@ -17874,7 +17965,7 @@
         <v>4</v>
       </c>
       <c r="G242">
-        <v>0.28999999999999998</v>
+        <v>0.19</v>
       </c>
       <c r="H242">
         <v>168</v>
@@ -17883,19 +17974,19 @@
         <v>3</v>
       </c>
       <c r="AK242">
-        <v>0.28999999999999998</v>
+        <v>0.19</v>
       </c>
       <c r="AL242" s="1">
-        <v>7.1302718295753895E-2</v>
+        <v>7.5039513227729199E-2</v>
       </c>
       <c r="AM242" s="1">
-        <v>0.29856626366017802</v>
+        <v>0.192337169219545</v>
       </c>
       <c r="AN242" s="1">
         <v>7.7849894416152296E-2</v>
       </c>
       <c r="AO242" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="AP242" t="s">
         <v>6</v>
@@ -17913,12 +18004,12 @@
         <v>116</v>
       </c>
       <c r="BD242" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="243" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B243" t="s">
         <v>1</v>
@@ -17927,7 +18018,7 @@
         <v>1</v>
       </c>
       <c r="D243" t="s">
-        <v>404</v>
+        <v>293</v>
       </c>
       <c r="E243" t="s">
         <v>1</v>
@@ -17936,7 +18027,7 @@
         <v>4</v>
       </c>
       <c r="G243">
-        <v>0.23</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H243">
         <v>168</v>
@@ -17945,19 +18036,19 @@
         <v>3</v>
       </c>
       <c r="AK243">
-        <v>0.23</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="AL243" s="1">
-        <v>7.3731635001537801E-2</v>
-      </c>
-      <c r="AM243">
-        <v>0.234189466759367</v>
+        <v>7.1302718295753895E-2</v>
+      </c>
+      <c r="AM243" s="1">
+        <v>0.29856626366017802</v>
       </c>
       <c r="AN243" s="1">
         <v>7.7849894416152296E-2</v>
       </c>
       <c r="AO243" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="AP243" t="s">
         <v>6</v>
@@ -17975,54 +18066,48 @@
         <v>116</v>
       </c>
       <c r="BD243" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="244" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="B244" t="s">
-        <v>406</v>
+        <v>1</v>
       </c>
       <c r="C244" t="s">
         <v>1</v>
       </c>
       <c r="D244" t="s">
-        <v>44</v>
+        <v>403</v>
       </c>
       <c r="E244" t="s">
         <v>1</v>
       </c>
       <c r="F244" t="s">
-        <v>19</v>
-      </c>
-      <c r="J244">
-        <v>0.521058574</v>
-      </c>
-      <c r="K244">
-        <v>0.15946897700000001</v>
-      </c>
-      <c r="L244">
-        <v>14</v>
-      </c>
-      <c r="M244">
-        <v>14</v>
-      </c>
-      <c r="N244">
+        <v>4</v>
+      </c>
+      <c r="G244">
+        <v>0.23</v>
+      </c>
+      <c r="H244">
+        <v>168</v>
+      </c>
+      <c r="I244">
         <v>3</v>
       </c>
       <c r="AK244">
-        <v>0.252113578984761</v>
-      </c>
-      <c r="AL244">
-        <v>0.18093690974440399</v>
+        <v>0.23</v>
+      </c>
+      <c r="AL244" s="1">
+        <v>7.3731635001537801E-2</v>
       </c>
       <c r="AM244">
-        <v>0.25766857135089799</v>
-      </c>
-      <c r="AN244">
-        <v>0.193218094659804</v>
+        <v>0.234189466759367</v>
+      </c>
+      <c r="AN244" s="1">
+        <v>7.7849894416152296E-2</v>
       </c>
       <c r="AO244" t="s">
         <v>26</v>
@@ -18031,30 +18116,27 @@
         <v>6</v>
       </c>
       <c r="AQ244" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="AR244" t="s">
         <v>8</v>
       </c>
       <c r="AS244">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AT244" t="s">
-        <v>9</v>
-      </c>
-      <c r="BC244" t="s">
-        <v>407</v>
+        <v>116</v>
       </c>
       <c r="BD244" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="245" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
+        <v>404</v>
+      </c>
+      <c r="B245" t="s">
         <v>405</v>
-      </c>
-      <c r="B245" t="s">
-        <v>409</v>
       </c>
       <c r="C245" t="s">
         <v>1</v>
@@ -18068,11 +18150,11 @@
       <c r="F245" t="s">
         <v>19</v>
       </c>
-      <c r="J245" s="2">
-        <v>1.3160066509999999</v>
+      <c r="J245">
+        <v>0.521058574</v>
       </c>
       <c r="K245">
-        <v>0.189713357</v>
+        <v>0.15946897700000001</v>
       </c>
       <c r="L245">
         <v>14</v>
@@ -18084,16 +18166,16 @@
         <v>3</v>
       </c>
       <c r="AK245">
-        <v>0.54967980997843602</v>
+        <v>0.252113578984761</v>
       </c>
       <c r="AL245">
-        <v>0.126959162679183</v>
+        <v>0.18093690974440399</v>
       </c>
       <c r="AM245">
-        <v>0.61792237562034202</v>
+        <v>0.25766857135089799</v>
       </c>
       <c r="AN245">
-        <v>0.18192846520956299</v>
+        <v>0.193218094659804</v>
       </c>
       <c r="AO245" t="s">
         <v>26</v>
@@ -18114,18 +18196,18 @@
         <v>9</v>
       </c>
       <c r="BC245" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="BD245" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="246" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B246" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C246" t="s">
         <v>1</v>
@@ -18139,32 +18221,32 @@
       <c r="F246" t="s">
         <v>19</v>
       </c>
-      <c r="J246">
-        <v>0.24728792099999999</v>
+      <c r="J246" s="2">
+        <v>1.3160066509999999</v>
       </c>
       <c r="K246">
-        <v>0.11859924199999999</v>
+        <v>0.189713357</v>
       </c>
       <c r="L246">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M246">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="N246">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK246">
-        <v>-0.122709537072517</v>
+        <v>0.54967980997843602</v>
       </c>
       <c r="AL246">
-        <v>0.168316693485384</v>
+        <v>0.126959162679183</v>
       </c>
       <c r="AM246">
-        <v>-0.12333106702734301</v>
+        <v>0.61792237562034202</v>
       </c>
       <c r="AN246">
-        <v>0.170889890307869</v>
+        <v>0.18192846520956299</v>
       </c>
       <c r="AO246" t="s">
         <v>26</v>
@@ -18185,18 +18267,18 @@
         <v>9</v>
       </c>
       <c r="BC246" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="BD246" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="247" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B247" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C247" t="s">
         <v>1</v>
@@ -18211,31 +18293,31 @@
         <v>19</v>
       </c>
       <c r="J247">
-        <v>0.44937575200000002</v>
+        <v>0.24728792099999999</v>
       </c>
       <c r="K247">
-        <v>0.10265044399999999</v>
+        <v>0.11859924199999999</v>
       </c>
       <c r="L247">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M247">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N247">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK247">
-        <v>0.21922232790873999</v>
+        <v>-0.122709537072517</v>
       </c>
       <c r="AL247">
-        <v>0.14878729886288</v>
+        <v>0.168316693485384</v>
       </c>
       <c r="AM247">
-        <v>0.22283902992136101</v>
+        <v>-0.12333106702734301</v>
       </c>
       <c r="AN247">
-        <v>0.156298772323787</v>
+        <v>0.170889890307869</v>
       </c>
       <c r="AO247" t="s">
         <v>26</v>
@@ -18256,18 +18338,18 @@
         <v>9</v>
       </c>
       <c r="BC247" t="s">
+        <v>411</v>
+      </c>
+      <c r="BD247" t="s">
         <v>407</v>
-      </c>
-      <c r="BD247" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="248" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B248" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C248" t="s">
         <v>1</v>
@@ -18282,31 +18364,31 @@
         <v>19</v>
       </c>
       <c r="J248">
-        <v>0.627600096</v>
+        <v>0.44937575200000002</v>
       </c>
       <c r="K248">
-        <v>0.123780168</v>
+        <v>0.10265044399999999</v>
       </c>
       <c r="L248">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M248">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="N248">
         <v>3</v>
       </c>
       <c r="AK248">
-        <v>0.29940483715614602</v>
+        <v>0.21922232790873999</v>
       </c>
       <c r="AL248">
-        <v>0.15279634250882601</v>
+        <v>0.14878729886288</v>
       </c>
       <c r="AM248">
-        <v>0.30886570730625501</v>
+        <v>0.22283902992136101</v>
       </c>
       <c r="AN248">
-        <v>0.16784227018902001</v>
+        <v>0.156298772323787</v>
       </c>
       <c r="AO248" t="s">
         <v>26</v>
@@ -18327,18 +18409,18 @@
         <v>9</v>
       </c>
       <c r="BC248" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="BD248" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="249" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B249" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C249" t="s">
         <v>1</v>
@@ -18353,31 +18435,31 @@
         <v>19</v>
       </c>
       <c r="J249">
-        <v>0.36363537600000001</v>
+        <v>0.627600096</v>
       </c>
       <c r="K249">
-        <v>0.14538706700000001</v>
+        <v>0.123780168</v>
       </c>
       <c r="L249">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M249">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="N249">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK249">
-        <v>-0.17888496789436301</v>
+        <v>0.29940483715614602</v>
       </c>
       <c r="AL249">
-        <v>0.18157081425836399</v>
+        <v>0.15279634250882601</v>
       </c>
       <c r="AM249">
-        <v>-0.18083055821648</v>
+        <v>0.30886570730625501</v>
       </c>
       <c r="AN249">
-        <v>0.18757312262091</v>
+        <v>0.16784227018902001</v>
       </c>
       <c r="AO249" t="s">
         <v>26</v>
@@ -18398,119 +18480,122 @@
         <v>9</v>
       </c>
       <c r="BC249" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="BD249" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="250" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="B250" t="s">
-        <v>1</v>
+        <v>414</v>
       </c>
       <c r="C250" t="s">
         <v>1</v>
       </c>
       <c r="D250" t="s">
-        <v>417</v>
+        <v>44</v>
       </c>
       <c r="E250" t="s">
         <v>1</v>
       </c>
       <c r="F250" t="s">
-        <v>4</v>
-      </c>
-      <c r="G250">
-        <v>0.24</v>
-      </c>
-      <c r="H250">
-        <v>234</v>
-      </c>
-      <c r="I250">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="J250">
+        <v>0.36363537600000001</v>
+      </c>
+      <c r="K250">
+        <v>0.14538706700000001</v>
+      </c>
+      <c r="L250">
+        <v>15</v>
+      </c>
+      <c r="M250">
+        <v>15</v>
+      </c>
+      <c r="N250">
+        <v>2</v>
       </c>
       <c r="AK250">
-        <v>0.24</v>
-      </c>
-      <c r="AL250" s="1">
-        <v>6.2005367733008597E-2</v>
+        <v>-0.17888496789436301</v>
+      </c>
+      <c r="AL250">
+        <v>0.18157081425836399</v>
       </c>
       <c r="AM250">
-        <v>0.244774112659353</v>
-      </c>
-      <c r="AN250" s="1">
-        <v>6.5795169495976899E-2</v>
+        <v>-0.18083055821648</v>
+      </c>
+      <c r="AN250">
+        <v>0.18757312262091</v>
       </c>
       <c r="AO250" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="AP250" t="s">
         <v>6</v>
       </c>
       <c r="AQ250" t="s">
-        <v>115</v>
+        <v>7</v>
       </c>
       <c r="AR250" t="s">
         <v>8</v>
       </c>
       <c r="AS250">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AT250" t="s">
-        <v>116</v>
+        <v>9</v>
+      </c>
+      <c r="BC250" t="s">
+        <v>411</v>
       </c>
       <c r="BD250" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
     </row>
     <row r="251" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B251" t="s">
         <v>1</v>
       </c>
       <c r="C251" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D251" t="s">
-        <v>263</v>
+        <v>416</v>
       </c>
       <c r="E251" t="s">
         <v>1</v>
       </c>
       <c r="F251" t="s">
-        <v>19</v>
-      </c>
-      <c r="J251">
-        <v>0.44</v>
-      </c>
-      <c r="K251">
-        <v>2.7311999999999999E-2</v>
-      </c>
-      <c r="L251">
-        <v>75</v>
-      </c>
-      <c r="M251">
-        <v>75</v>
-      </c>
-      <c r="N251">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G251">
+        <v>0.24</v>
+      </c>
+      <c r="H251">
+        <v>234</v>
+      </c>
+      <c r="I251">
+        <v>3</v>
       </c>
       <c r="AK251">
-        <v>0.21486178267511999</v>
-      </c>
-      <c r="AL251">
-        <v>7.6976159209578995E-2</v>
+        <v>0.24</v>
+      </c>
+      <c r="AL251" s="1">
+        <v>6.2005367733008597E-2</v>
       </c>
       <c r="AM251">
-        <v>0.218262907439882</v>
+        <v>0.244774112659353</v>
       </c>
       <c r="AN251" s="1">
-        <v>8.0701805315322603E-2</v>
+        <v>6.5795169495976899E-2</v>
       </c>
       <c r="AO251" t="s">
         <v>5</v>
@@ -18519,24 +18604,24 @@
         <v>6</v>
       </c>
       <c r="AQ251" t="s">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="AR251" t="s">
         <v>8</v>
       </c>
       <c r="AS251">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AT251" t="s">
         <v>116</v>
       </c>
       <c r="BD251" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="252" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B252" t="s">
         <v>1</v>
@@ -18545,7 +18630,7 @@
         <v>2</v>
       </c>
       <c r="D252" t="s">
-        <v>421</v>
+        <v>263</v>
       </c>
       <c r="E252" t="s">
         <v>1</v>
@@ -18554,10 +18639,10 @@
         <v>19</v>
       </c>
       <c r="J252">
-        <v>-0.39</v>
+        <v>0.44</v>
       </c>
       <c r="K252">
-        <v>2.7173666999999999E-2</v>
+        <v>2.7311999999999999E-2</v>
       </c>
       <c r="L252">
         <v>75</v>
@@ -18566,25 +18651,25 @@
         <v>75</v>
       </c>
       <c r="N252">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK252">
-        <v>0.191395051403356</v>
-      </c>
-      <c r="AL252" s="1">
-        <v>7.7934976527938807E-2</v>
+        <v>0.21486178267511999</v>
+      </c>
+      <c r="AL252">
+        <v>7.6976159209578995E-2</v>
       </c>
       <c r="AM252">
-        <v>0.19378486722187599</v>
+        <v>0.218262907439882</v>
       </c>
       <c r="AN252" s="1">
-        <v>8.0898454010413706E-2</v>
+        <v>8.0701805315322603E-2</v>
       </c>
       <c r="AO252" t="s">
         <v>5</v>
       </c>
       <c r="AP252" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="AQ252" t="s">
         <v>7</v>
@@ -18599,12 +18684,12 @@
         <v>116</v>
       </c>
       <c r="BD252" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="253" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B253" t="s">
         <v>1</v>
@@ -18613,7 +18698,7 @@
         <v>2</v>
       </c>
       <c r="D253" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E253" t="s">
         <v>1</v>
@@ -18622,31 +18707,31 @@
         <v>19</v>
       </c>
       <c r="J253">
-        <v>7.0000000000000007E-2</v>
+        <v>-0.39</v>
       </c>
       <c r="K253">
-        <v>3.4503879000000001E-2</v>
+        <v>2.7173666999999999E-2</v>
       </c>
       <c r="L253">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="M253">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="N253">
-        <v>1</v>
-      </c>
-      <c r="AK253" s="1">
-        <v>3.4978582175618597E-2</v>
+        <v>3</v>
+      </c>
+      <c r="AK253">
+        <v>0.191395051403356</v>
       </c>
       <c r="AL253" s="1">
-        <v>9.2705700034930505E-2</v>
-      </c>
-      <c r="AM253" s="1">
-        <v>3.4992858102937403E-2</v>
+        <v>7.7934976527938807E-2</v>
+      </c>
+      <c r="AM253">
+        <v>0.19378486722187599</v>
       </c>
       <c r="AN253" s="1">
-        <v>9.2819264517473299E-2</v>
+        <v>8.0898454010413706E-2</v>
       </c>
       <c r="AO253" t="s">
         <v>5</v>
@@ -18667,12 +18752,12 @@
         <v>116</v>
       </c>
       <c r="BD253" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="254" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B254" t="s">
         <v>1</v>
@@ -18681,7 +18766,7 @@
         <v>2</v>
       </c>
       <c r="D254" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E254" t="s">
         <v>1</v>
@@ -18690,31 +18775,31 @@
         <v>19</v>
       </c>
       <c r="J254">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K254">
-        <v>2.6700000000000002E-2</v>
+        <v>3.4503879000000001E-2</v>
       </c>
       <c r="L254">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="M254">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="N254">
         <v>1</v>
       </c>
       <c r="AK254" s="1">
-        <v>4.9937616943892198E-2</v>
+        <v>3.4978582175618597E-2</v>
       </c>
       <c r="AL254" s="1">
-        <v>8.1395250312464404E-2</v>
+        <v>9.2705700034930505E-2</v>
       </c>
       <c r="AM254" s="1">
-        <v>4.99791900693487E-2</v>
+        <v>3.4992858102937403E-2</v>
       </c>
       <c r="AN254" s="1">
-        <v>8.1598738438245597E-2</v>
+        <v>9.2819264517473299E-2</v>
       </c>
       <c r="AO254" t="s">
         <v>5</v>
@@ -18735,74 +18820,80 @@
         <v>116</v>
       </c>
       <c r="BD254" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="255" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="B255" t="s">
         <v>1</v>
       </c>
       <c r="C255" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D255" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E255" t="s">
         <v>1</v>
       </c>
       <c r="F255" t="s">
-        <v>4</v>
-      </c>
-      <c r="G255">
-        <v>0.24</v>
-      </c>
-      <c r="H255">
-        <v>1492</v>
-      </c>
-      <c r="I255">
-        <v>3</v>
-      </c>
-      <c r="AK255">
-        <v>0.24</v>
+        <v>19</v>
+      </c>
+      <c r="J255">
+        <v>0.1</v>
+      </c>
+      <c r="K255">
+        <v>2.6700000000000002E-2</v>
+      </c>
+      <c r="L255">
+        <v>75</v>
+      </c>
+      <c r="M255">
+        <v>75</v>
+      </c>
+      <c r="N255">
+        <v>1</v>
+      </c>
+      <c r="AK255" s="1">
+        <v>4.9937616943892198E-2</v>
       </c>
       <c r="AL255" s="1">
-        <v>2.44223768623184E-2</v>
-      </c>
-      <c r="AM255">
-        <v>0.244774112659353</v>
+        <v>8.1395250312464404E-2</v>
+      </c>
+      <c r="AM255" s="1">
+        <v>4.99791900693487E-2</v>
       </c>
       <c r="AN255" s="1">
-        <v>2.5915085804667198E-2</v>
+        <v>8.1598738438245597E-2</v>
       </c>
       <c r="AO255" t="s">
         <v>5</v>
       </c>
       <c r="AP255" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="AQ255" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="AR255" t="s">
         <v>8</v>
       </c>
       <c r="AS255">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT255" t="s">
         <v>116</v>
       </c>
       <c r="BD255" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="256" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B256" t="s">
         <v>1</v>
@@ -18811,7 +18902,7 @@
         <v>1</v>
       </c>
       <c r="D256" t="s">
-        <v>245</v>
+        <v>424</v>
       </c>
       <c r="E256" t="s">
         <v>1</v>
@@ -18820,28 +18911,28 @@
         <v>4</v>
       </c>
       <c r="G256">
-        <v>0.28000000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="H256">
-        <v>795</v>
+        <v>1492</v>
       </c>
       <c r="I256">
         <v>3</v>
       </c>
       <c r="AK256">
-        <v>0.28000000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="AL256" s="1">
-        <v>3.2747630032221801E-2</v>
+        <v>2.44223768623184E-2</v>
       </c>
       <c r="AM256">
-        <v>0.28768207245178101</v>
+        <v>0.244774112659353</v>
       </c>
       <c r="AN256" s="1">
-        <v>3.5533452725935097E-2</v>
+        <v>2.5915085804667198E-2</v>
       </c>
       <c r="AO256" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AP256" t="s">
         <v>6</v>
@@ -18859,12 +18950,12 @@
         <v>116</v>
       </c>
       <c r="BD256" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="257" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B257" t="s">
         <v>1</v>
@@ -18873,7 +18964,7 @@
         <v>1</v>
       </c>
       <c r="D257" t="s">
-        <v>428</v>
+        <v>245</v>
       </c>
       <c r="E257" t="s">
         <v>1</v>
@@ -18882,7 +18973,7 @@
         <v>4</v>
       </c>
       <c r="G257">
-        <v>-0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H257">
         <v>795</v>
@@ -18891,13 +18982,13 @@
         <v>3</v>
       </c>
       <c r="AK257">
-        <v>0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AL257" s="1">
-        <v>3.3813633613999798E-2</v>
+        <v>3.2747630032221801E-2</v>
       </c>
       <c r="AM257">
-        <v>0.223656109021832</v>
+        <v>0.28768207245178101</v>
       </c>
       <c r="AN257" s="1">
         <v>3.5533452725935097E-2</v>
@@ -18921,21 +19012,21 @@
         <v>116</v>
       </c>
       <c r="BD257" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="258" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
+        <v>426</v>
+      </c>
+      <c r="B258" t="s">
+        <v>1</v>
+      </c>
+      <c r="C258" t="s">
+        <v>1</v>
+      </c>
+      <c r="D258" t="s">
         <v>427</v>
-      </c>
-      <c r="B258" t="s">
-        <v>1</v>
-      </c>
-      <c r="C258" t="s">
-        <v>1</v>
-      </c>
-      <c r="D258" t="s">
-        <v>430</v>
       </c>
       <c r="E258" t="s">
         <v>1</v>
@@ -18944,7 +19035,7 @@
         <v>4</v>
       </c>
       <c r="G258">
-        <v>0.19</v>
+        <v>-0.22</v>
       </c>
       <c r="H258">
         <v>795</v>
@@ -18953,13 +19044,13 @@
         <v>3</v>
       </c>
       <c r="AK258">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="AL258" s="1">
-        <v>3.4250695082528801E-2</v>
+        <v>3.3813633613999798E-2</v>
       </c>
       <c r="AM258">
-        <v>0.192337169219545</v>
+        <v>0.223656109021832</v>
       </c>
       <c r="AN258" s="1">
         <v>3.5533452725935097E-2</v>
@@ -18983,12 +19074,12 @@
         <v>116</v>
       </c>
       <c r="BD258" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="259" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B259" t="s">
         <v>1</v>
@@ -18997,7 +19088,7 @@
         <v>1</v>
       </c>
       <c r="D259" t="s">
-        <v>293</v>
+        <v>429</v>
       </c>
       <c r="E259" t="s">
         <v>1</v>
@@ -19006,7 +19097,7 @@
         <v>4</v>
       </c>
       <c r="G259">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="H259">
         <v>795</v>
@@ -19015,19 +19106,19 @@
         <v>3</v>
       </c>
       <c r="AK259">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="AL259" s="1">
-        <v>3.5178118198675702E-2</v>
-      </c>
-      <c r="AM259" s="1">
-        <v>0.100335347731076</v>
+        <v>3.4250695082528801E-2</v>
+      </c>
+      <c r="AM259">
+        <v>0.192337169219545</v>
       </c>
       <c r="AN259" s="1">
         <v>3.5533452725935097E-2</v>
       </c>
       <c r="AO259" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AP259" t="s">
         <v>6</v>
@@ -19045,11 +19136,70 @@
         <v>116</v>
       </c>
       <c r="BD259" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="260" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="AN260" s="1"/>
+      <c r="A260" t="s">
+        <v>426</v>
+      </c>
+      <c r="B260" t="s">
+        <v>1</v>
+      </c>
+      <c r="C260" t="s">
+        <v>1</v>
+      </c>
+      <c r="D260" t="s">
+        <v>293</v>
+      </c>
+      <c r="E260" t="s">
+        <v>1</v>
+      </c>
+      <c r="F260" t="s">
+        <v>4</v>
+      </c>
+      <c r="G260">
+        <v>0.1</v>
+      </c>
+      <c r="H260">
+        <v>795</v>
+      </c>
+      <c r="I260">
+        <v>3</v>
+      </c>
+      <c r="AK260">
+        <v>0.1</v>
+      </c>
+      <c r="AL260" s="1">
+        <v>3.5178118198675702E-2</v>
+      </c>
+      <c r="AM260" s="1">
+        <v>0.100335347731076</v>
+      </c>
+      <c r="AN260" s="1">
+        <v>3.5533452725935097E-2</v>
+      </c>
+      <c r="AO260" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP260" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ260" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR260" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS260">
+        <v>3</v>
+      </c>
+      <c r="AT260" t="s">
+        <v>116</v>
+      </c>
+      <c r="BD260" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="261" spans="1:56" x14ac:dyDescent="0.25">
       <c r="AN261" s="1"/>
@@ -19072,8 +19222,8 @@
     <row r="267" spans="1:56" x14ac:dyDescent="0.25">
       <c r="AN267" s="1"/>
     </row>
-    <row r="270" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="AN270" s="1"/>
+    <row r="268" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AN268" s="1"/>
     </row>
     <row r="271" spans="1:56" x14ac:dyDescent="0.25">
       <c r="AN271" s="1"/>
@@ -19183,8 +19333,8 @@
     <row r="306" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN306" s="1"/>
     </row>
-    <row r="310" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN310" s="1"/>
+    <row r="307" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN307" s="1"/>
     </row>
     <row r="311" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN311" s="1"/>
@@ -19192,11 +19342,11 @@
     <row r="312" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN312" s="1"/>
     </row>
-    <row r="341" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN341" s="1"/>
-    </row>
-    <row r="364" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN364" s="1"/>
+    <row r="313" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN313" s="1"/>
+    </row>
+    <row r="342" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN342" s="1"/>
     </row>
     <row r="365" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN365" s="1"/>
@@ -19207,8 +19357,11 @@
     <row r="367" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN367" s="1"/>
     </row>
+    <row r="368" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN368" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AT368">
+  <autoFilter ref="A1:AT369">
     <sortState ref="A2:AV391">
       <sortCondition ref="A1:A391"/>
     </sortState>

</xml_diff>

<commit_message>
Added some effect sizes from Sestir and Bartholow. -Math file included.
</commit_message>
<xml_diff>
--- a/edited_data.xlsx
+++ b/edited_data.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhilgard\Documents\GitHub\greietemeyer_meta\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12885"/>
   </bookViews>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AT$369</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3255" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3264" uniqueCount="508">
   <si>
     <t>Adachi, P. J. C., &amp; Willoughby, T. (2011). S1</t>
   </si>
@@ -1196,9 +1191,6 @@
     <t>Total state hostility</t>
   </si>
   <si>
-    <t>aggressive behaviour (0 min delay)</t>
-  </si>
-  <si>
     <t>Sestir, M. A., &amp; Bartholow, B. D. (2010). Violent and nonviolent video games produce opposing effects on aggressive and prosocial outcomes. Journal Of Experimental Social Psychology, 46(6), 934-942.</t>
   </si>
   <si>
@@ -1536,6 +1528,24 @@
   </si>
   <si>
     <t>Sestir, M. A., &amp; Bartholow, B. D. (2010). S3</t>
+  </si>
+  <si>
+    <t>0 min delay</t>
+  </si>
+  <si>
+    <t>15 min delay</t>
+  </si>
+  <si>
+    <t>Open for debate whether to include 0min delay only</t>
+  </si>
+  <si>
+    <t>mean intensity, CRTT</t>
+  </si>
+  <si>
+    <t>d = 0.5</t>
+  </si>
+  <si>
+    <t>d = 0.44</t>
   </si>
 </sst>
 </file>
@@ -1650,7 +1660,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1685,7 +1695,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1862,7 +1872,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1872,9 +1882,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD368"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF224" sqref="AF224"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AK235" sqref="AK235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,9 +1892,8 @@
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="31" width="19.42578125" hidden="1" customWidth="1"/>
-    <col min="32" max="33" width="19.42578125" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="33" width="19.42578125" customWidth="1"/>
     <col min="34" max="36" width="9.140625" customWidth="1"/>
     <col min="40" max="40" width="12" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="85.5703125" bestFit="1" customWidth="1"/>
@@ -1892,172 +1901,172 @@
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B1" t="s">
         <v>431</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>432</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>433</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>434</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>435</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H1" t="s">
+        <v>448</v>
+      </c>
+      <c r="I1" t="s">
+        <v>449</v>
+      </c>
+      <c r="J1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K1" t="s">
+        <v>451</v>
+      </c>
+      <c r="L1" t="s">
+        <v>452</v>
+      </c>
+      <c r="M1" t="s">
+        <v>453</v>
+      </c>
+      <c r="N1" t="s">
+        <v>454</v>
+      </c>
+      <c r="O1" t="s">
+        <v>455</v>
+      </c>
+      <c r="P1" t="s">
+        <v>459</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>456</v>
+      </c>
+      <c r="R1" t="s">
+        <v>457</v>
+      </c>
+      <c r="S1" t="s">
+        <v>458</v>
+      </c>
+      <c r="T1" t="s">
+        <v>460</v>
+      </c>
+      <c r="U1" t="s">
+        <v>461</v>
+      </c>
+      <c r="V1" t="s">
+        <v>462</v>
+      </c>
+      <c r="W1" t="s">
+        <v>463</v>
+      </c>
+      <c r="X1" t="s">
+        <v>464</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>465</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>466</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>467</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>468</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>469</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>470</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>471</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>472</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>473</v>
+      </c>
+      <c r="AH1" t="s">
         <v>436</v>
       </c>
-      <c r="G1" t="s">
-        <v>448</v>
-      </c>
-      <c r="H1" t="s">
-        <v>449</v>
-      </c>
-      <c r="I1" t="s">
-        <v>450</v>
-      </c>
-      <c r="J1" t="s">
-        <v>451</v>
-      </c>
-      <c r="K1" t="s">
-        <v>452</v>
-      </c>
-      <c r="L1" t="s">
-        <v>453</v>
-      </c>
-      <c r="M1" t="s">
-        <v>454</v>
-      </c>
-      <c r="N1" t="s">
-        <v>455</v>
-      </c>
-      <c r="O1" t="s">
-        <v>456</v>
-      </c>
-      <c r="P1" t="s">
-        <v>460</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>457</v>
-      </c>
-      <c r="R1" t="s">
-        <v>458</v>
-      </c>
-      <c r="S1" t="s">
-        <v>459</v>
-      </c>
-      <c r="T1" t="s">
-        <v>461</v>
-      </c>
-      <c r="U1" t="s">
-        <v>462</v>
-      </c>
-      <c r="V1" t="s">
-        <v>463</v>
-      </c>
-      <c r="W1" t="s">
-        <v>464</v>
-      </c>
-      <c r="X1" t="s">
-        <v>465</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>466</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>467</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>468</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>469</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>470</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>471</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>472</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>473</v>
-      </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>474</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
+        <v>475</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>445</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>446</v>
+      </c>
+      <c r="AM1" t="s">
         <v>437</v>
       </c>
-      <c r="AI1" t="s">
-        <v>475</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="AN1" t="s">
+        <v>438</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>439</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>440</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>441</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>442</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>443</v>
+      </c>
+      <c r="AT1" t="s">
         <v>476</v>
       </c>
-      <c r="AK1" t="s">
-        <v>446</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>447</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>438</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>439</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>440</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>441</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>442</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>443</v>
-      </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
+        <v>484</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>485</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>486</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>487</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>480</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>481</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>482</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>483</v>
+      </c>
+      <c r="BC1" t="s">
         <v>444</v>
       </c>
-      <c r="AT1" t="s">
-        <v>477</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>485</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>486</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>487</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>488</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>481</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>482</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>483</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>484</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>445</v>
-      </c>
       <c r="BD1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
@@ -2538,7 +2547,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J9">
         <f>AVERAGE(0.44, 0.5)</f>
@@ -2587,19 +2596,19 @@
         <v>9</v>
       </c>
       <c r="AU9" t="s">
+        <v>488</v>
+      </c>
+      <c r="AV9" t="s">
         <v>489</v>
       </c>
-      <c r="AV9" t="s">
+      <c r="AY9" t="s">
+        <v>506</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>507</v>
+      </c>
+      <c r="BC9" t="s">
         <v>490</v>
-      </c>
-      <c r="AY9">
-        <v>0.5</v>
-      </c>
-      <c r="AZ9">
-        <v>0.44</v>
-      </c>
-      <c r="BC9" t="s">
-        <v>491</v>
       </c>
       <c r="BD9" t="s">
         <v>22</v>
@@ -2959,7 +2968,7 @@
         <v>87</v>
       </c>
       <c r="U15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK15">
         <v>0.11775505103579501</v>
@@ -3033,7 +3042,7 @@
         <v>87</v>
       </c>
       <c r="U16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK16" s="1">
         <v>1.88132384358922E-2</v>
@@ -3107,7 +3116,7 @@
         <v>87</v>
       </c>
       <c r="U17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK17">
         <v>0.105854786920116</v>
@@ -3181,7 +3190,7 @@
         <v>23</v>
       </c>
       <c r="U18" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK18">
         <v>0.38708835994406798</v>
@@ -3255,7 +3264,7 @@
         <v>23</v>
       </c>
       <c r="U19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK19">
         <v>0.37324680142328898</v>
@@ -3329,7 +3338,7 @@
         <v>22</v>
       </c>
       <c r="U20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK20">
         <v>0.29530730609491901</v>
@@ -3403,7 +3412,7 @@
         <v>23</v>
       </c>
       <c r="U21" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK21">
         <v>0.157908384915591</v>
@@ -3808,7 +3817,7 @@
         <v>18</v>
       </c>
       <c r="U27" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK27">
         <v>-0.32001329437029802</v>
@@ -3885,7 +3894,7 @@
         <v>18</v>
       </c>
       <c r="U28" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK28">
         <v>0.368305806793924</v>
@@ -4027,7 +4036,7 @@
         <v>41</v>
       </c>
       <c r="U30" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK30" s="1">
         <v>6.5745978697184806E-2</v>
@@ -4101,7 +4110,7 @@
         <v>41</v>
       </c>
       <c r="U31" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK31" s="1">
         <v>1.47224692839925E-2</v>
@@ -4485,7 +4494,7 @@
         <v>18</v>
       </c>
       <c r="U37" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK37">
         <v>0.23238050000631399</v>
@@ -4559,7 +4568,7 @@
         <v>18</v>
       </c>
       <c r="U38" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK38">
         <v>-0.16973737763046201</v>
@@ -4831,7 +4840,7 @@
         <v>29</v>
       </c>
       <c r="U42" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK42">
         <v>-0.191538071371774</v>
@@ -4905,7 +4914,7 @@
         <v>29</v>
       </c>
       <c r="U43" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK43">
         <v>0.14730956928116101</v>
@@ -4979,7 +4988,7 @@
         <v>29</v>
       </c>
       <c r="U44" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK44" s="1">
         <v>-1.00046436056182E-2</v>
@@ -6494,7 +6503,7 @@
         <v>25</v>
       </c>
       <c r="U68" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK68">
         <v>3.5154698054722003E-2</v>
@@ -6568,7 +6577,7 @@
         <v>26</v>
       </c>
       <c r="U69" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK69">
         <v>-0.11588005146689299</v>
@@ -6642,7 +6651,7 @@
         <v>25</v>
       </c>
       <c r="U70" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK70" s="1">
         <v>3.1836903298351697E-2</v>
@@ -6716,7 +6725,7 @@
         <v>26</v>
       </c>
       <c r="U71" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AK71">
         <v>-0.11565463171158399</v>
@@ -6982,7 +6991,7 @@
         <v>13</v>
       </c>
       <c r="U75" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK75">
         <v>0.43481823629979299</v>
@@ -7186,7 +7195,7 @@
         <v>37</v>
       </c>
       <c r="U78" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK78">
         <v>0.30197010641017102</v>
@@ -8090,7 +8099,7 @@
         <v>169</v>
       </c>
       <c r="U92" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK92">
         <v>0.14788611324801701</v>
@@ -10119,7 +10128,7 @@
         <v>38</v>
       </c>
       <c r="U124" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK124">
         <v>0.20307294859175301</v>
@@ -10193,7 +10202,7 @@
         <v>21</v>
       </c>
       <c r="U125" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK125">
         <v>0.359136094885042</v>
@@ -10391,7 +10400,7 @@
         <v>20</v>
       </c>
       <c r="U128" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK128" s="1">
         <v>-1.22028373675277E-2</v>
@@ -10465,7 +10474,7 @@
         <v>20</v>
       </c>
       <c r="U129" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK129">
         <v>0.45471427033982198</v>
@@ -10539,7 +10548,7 @@
         <v>20</v>
       </c>
       <c r="U130" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK130">
         <v>0.73201968270769102</v>
@@ -10613,7 +10622,7 @@
         <v>20</v>
       </c>
       <c r="U131" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK131">
         <v>0.63694371197226296</v>
@@ -11024,7 +11033,7 @@
         <v>8</v>
       </c>
       <c r="U137" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK137">
         <v>0.40584569331961901</v>
@@ -11358,7 +11367,7 @@
         <v>42</v>
       </c>
       <c r="U142" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK142">
         <v>0.22443290236982399</v>
@@ -11692,7 +11701,7 @@
         <v>57</v>
       </c>
       <c r="U147" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK147">
         <v>0.15768945703450199</v>
@@ -11828,7 +11837,7 @@
         <v>9</v>
       </c>
       <c r="U149" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK149" s="1">
         <v>9.78372160424551E-2</v>
@@ -11902,7 +11911,7 @@
         <v>34</v>
       </c>
       <c r="U150" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK150">
         <v>-2.6005845470728001E-2</v>
@@ -11976,7 +11985,7 @@
         <v>34</v>
       </c>
       <c r="U151" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK151">
         <v>0.18219642438814199</v>
@@ -12050,7 +12059,7 @@
         <v>34</v>
       </c>
       <c r="U152" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AK152" s="1">
         <v>-8.1130243527845203E-2</v>
@@ -13541,13 +13550,13 @@
         <v>2</v>
       </c>
       <c r="D176" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E176" t="s">
         <v>1</v>
       </c>
       <c r="F176" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AF176">
         <v>153</v>
@@ -13580,7 +13589,7 @@
         <v>3</v>
       </c>
       <c r="BC176" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="BD176" t="s">
         <v>310</v>
@@ -13597,13 +13606,13 @@
         <v>2</v>
       </c>
       <c r="D177" t="s">
+        <v>492</v>
+      </c>
+      <c r="E177" t="s">
+        <v>1</v>
+      </c>
+      <c r="F177" t="s">
         <v>493</v>
-      </c>
-      <c r="E177" t="s">
-        <v>1</v>
-      </c>
-      <c r="F177" t="s">
-        <v>494</v>
       </c>
       <c r="AF177">
         <v>153</v>
@@ -13636,13 +13645,13 @@
         <v>3</v>
       </c>
       <c r="AU177" t="s">
+        <v>496</v>
+      </c>
+      <c r="AV177" t="s">
         <v>497</v>
       </c>
-      <c r="AV177" t="s">
-        <v>498</v>
-      </c>
       <c r="BC177" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="BD177" t="s">
         <v>310</v>
@@ -13665,7 +13674,7 @@
         <v>1</v>
       </c>
       <c r="F178" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AF178">
         <v>153</v>
@@ -13698,7 +13707,7 @@
         <v>3</v>
       </c>
       <c r="BC178" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="BD178" t="s">
         <v>310</v>
@@ -13946,7 +13955,7 @@
         <v>26</v>
       </c>
       <c r="U182" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK182">
         <v>0.204869051416882</v>
@@ -14020,7 +14029,7 @@
         <v>26</v>
       </c>
       <c r="U183" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK183">
         <v>0.48413896698103398</v>
@@ -14094,7 +14103,7 @@
         <v>26</v>
       </c>
       <c r="U184" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK184">
         <v>0.177114366993189</v>
@@ -14168,7 +14177,7 @@
         <v>26</v>
       </c>
       <c r="U185" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK185">
         <v>0.39554761159184498</v>
@@ -14242,7 +14251,7 @@
         <v>26</v>
       </c>
       <c r="U186" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK186">
         <v>0.165623109821497</v>
@@ -14316,7 +14325,7 @@
         <v>26</v>
       </c>
       <c r="U187" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK187">
         <v>0.38899447096877698</v>
@@ -14452,7 +14461,7 @@
         <v>542</v>
       </c>
       <c r="U189" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK189">
         <v>0.13385924414716799</v>
@@ -14526,7 +14535,7 @@
         <v>540</v>
       </c>
       <c r="U190" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK190">
         <v>0.18823993670091901</v>
@@ -15840,7 +15849,7 @@
         <v>59</v>
       </c>
       <c r="U211" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK211" s="1">
         <v>5.1455950994510703E-2</v>
@@ -16700,7 +16709,7 @@
         <v>84</v>
       </c>
       <c r="U224" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK224">
         <v>0.43045215970323403</v>
@@ -16774,7 +16783,7 @@
         <v>84</v>
       </c>
       <c r="U225" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AK225">
         <v>0.241289668231458</v>
@@ -17356,7 +17365,7 @@
     </row>
     <row r="234" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>1</v>
@@ -17365,7 +17374,7 @@
         <v>2</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>389</v>
+        <v>505</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>1</v>
@@ -17408,22 +17417,24 @@
       <c r="AC234" s="3"/>
       <c r="AD234" s="3"/>
       <c r="AE234" s="3"/>
-      <c r="AF234" s="3"/>
+      <c r="AF234" s="3">
+        <v>347</v>
+      </c>
       <c r="AG234" s="3"/>
       <c r="AH234" s="3"/>
       <c r="AI234" s="3"/>
       <c r="AJ234" s="3"/>
       <c r="AK234">
-        <v>0.196113257100091</v>
+        <v>0.15505360000000001</v>
       </c>
       <c r="AL234" s="1">
-        <v>4.8280239443733601E-2</v>
+        <v>5.2403230000000002E-2</v>
       </c>
       <c r="AM234">
-        <v>0.19868711719138199</v>
+        <v>0.1563145</v>
       </c>
       <c r="AN234">
-        <v>5.0211390073050997E-2</v>
+        <v>5.3694119999999998E-2</v>
       </c>
       <c r="AO234" t="s">
         <v>5</v>
@@ -17443,13 +17454,25 @@
       <c r="AT234" t="s">
         <v>9</v>
       </c>
+      <c r="AU234" t="s">
+        <v>502</v>
+      </c>
+      <c r="AV234" t="s">
+        <v>503</v>
+      </c>
+      <c r="AY234">
+        <v>0.15505360000000001</v>
+      </c>
+      <c r="AZ234">
+        <v>-1.8762669999999999E-2</v>
+      </c>
       <c r="BD234" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="235" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B235" s="3" t="s">
         <v>1</v>
@@ -17497,22 +17520,24 @@
       <c r="AC235" s="3"/>
       <c r="AD235" s="3"/>
       <c r="AE235" s="3"/>
-      <c r="AF235" s="3"/>
+      <c r="AF235" s="3">
+        <v>181</v>
+      </c>
       <c r="AG235" s="3"/>
       <c r="AH235" s="3"/>
       <c r="AI235" s="3"/>
       <c r="AJ235" s="3"/>
       <c r="AK235">
-        <v>0.11</v>
+        <v>0.1076838</v>
       </c>
       <c r="AL235" s="1">
         <v>7.4046235555901105E-2</v>
       </c>
       <c r="AM235">
-        <v>0.11044691579009699</v>
+        <v>0.108103</v>
       </c>
       <c r="AN235" s="1">
-        <v>7.4953168899586101E-2</v>
+        <v>7.495317E-2</v>
       </c>
       <c r="AO235" t="s">
         <v>20</v>
@@ -17532,13 +17557,28 @@
       <c r="AT235" t="s">
         <v>9</v>
       </c>
+      <c r="AU235" t="s">
+        <v>502</v>
+      </c>
+      <c r="AV235" t="s">
+        <v>503</v>
+      </c>
+      <c r="AY235">
+        <v>0.31958170000000002</v>
+      </c>
+      <c r="AZ235">
+        <v>-0.12746953</v>
+      </c>
+      <c r="BC235" t="s">
+        <v>504</v>
+      </c>
       <c r="BD235" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="236" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B236" s="3" t="s">
         <v>1</v>
@@ -17547,7 +17587,7 @@
         <v>2</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E236" s="3" t="s">
         <v>1</v>
@@ -17586,22 +17626,24 @@
       <c r="AC236" s="3"/>
       <c r="AD236" s="3"/>
       <c r="AE236" s="3"/>
-      <c r="AF236" s="3"/>
+      <c r="AF236" s="3">
+        <v>181</v>
+      </c>
       <c r="AG236" s="3"/>
       <c r="AH236" s="3"/>
       <c r="AI236" s="3"/>
       <c r="AJ236" s="3"/>
       <c r="AK236">
-        <v>0.21</v>
+        <v>0.21786530000000001</v>
       </c>
       <c r="AL236" s="1">
         <v>7.1647734151114403E-2</v>
       </c>
       <c r="AM236">
-        <v>0.21317134656486</v>
+        <v>0.2214139</v>
       </c>
       <c r="AN236" s="1">
-        <v>7.4953168899586101E-2</v>
+        <v>7.5377840000000002E-2</v>
       </c>
       <c r="AO236" t="s">
         <v>26</v>
@@ -17621,13 +17663,25 @@
       <c r="AT236" t="s">
         <v>9</v>
       </c>
+      <c r="AU236" t="s">
+        <v>502</v>
+      </c>
+      <c r="AV236" t="s">
+        <v>503</v>
+      </c>
+      <c r="AY236">
+        <v>0.40405380000000002</v>
+      </c>
+      <c r="AZ236">
+        <v>0</v>
+      </c>
       <c r="BD236" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="237" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B237" s="3" t="s">
         <v>1</v>
@@ -17636,7 +17690,7 @@
         <v>2</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E237" s="3" t="s">
         <v>1</v>
@@ -17675,16 +17729,16 @@
     </row>
     <row r="238" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
+        <v>392</v>
+      </c>
+      <c r="B238" t="s">
+        <v>1</v>
+      </c>
+      <c r="C238" t="s">
+        <v>2</v>
+      </c>
+      <c r="D238" t="s">
         <v>393</v>
-      </c>
-      <c r="B238" t="s">
-        <v>1</v>
-      </c>
-      <c r="C238" t="s">
-        <v>2</v>
-      </c>
-      <c r="D238" t="s">
-        <v>394</v>
       </c>
       <c r="E238" t="s">
         <v>1</v>
@@ -17738,21 +17792,21 @@
         <v>116</v>
       </c>
       <c r="BD238" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="239" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
+        <v>395</v>
+      </c>
+      <c r="B239" t="s">
+        <v>1</v>
+      </c>
+      <c r="C239" t="s">
+        <v>2</v>
+      </c>
+      <c r="D239" t="s">
         <v>396</v>
-      </c>
-      <c r="B239" t="s">
-        <v>1</v>
-      </c>
-      <c r="C239" t="s">
-        <v>2</v>
-      </c>
-      <c r="D239" t="s">
-        <v>397</v>
       </c>
       <c r="E239" t="s">
         <v>1</v>
@@ -17806,12 +17860,12 @@
         <v>116</v>
       </c>
       <c r="BD239" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="240" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B240" t="s">
         <v>1</v>
@@ -17874,12 +17928,12 @@
         <v>116</v>
       </c>
       <c r="BD240" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="241" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B241" t="s">
         <v>1</v>
@@ -17888,7 +17942,7 @@
         <v>2</v>
       </c>
       <c r="D241" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E241" t="s">
         <v>1</v>
@@ -17942,21 +17996,21 @@
         <v>116</v>
       </c>
       <c r="BD241" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="242" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
+        <v>399</v>
+      </c>
+      <c r="B242" t="s">
+        <v>1</v>
+      </c>
+      <c r="C242" t="s">
+        <v>1</v>
+      </c>
+      <c r="D242" t="s">
         <v>400</v>
-      </c>
-      <c r="B242" t="s">
-        <v>1</v>
-      </c>
-      <c r="C242" t="s">
-        <v>1</v>
-      </c>
-      <c r="D242" t="s">
-        <v>401</v>
       </c>
       <c r="E242" t="s">
         <v>1</v>
@@ -18004,12 +18058,12 @@
         <v>116</v>
       </c>
       <c r="BD242" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="243" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B243" t="s">
         <v>1</v>
@@ -18066,12 +18120,12 @@
         <v>116</v>
       </c>
       <c r="BD243" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="244" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B244" t="s">
         <v>1</v>
@@ -18080,7 +18134,7 @@
         <v>1</v>
       </c>
       <c r="D244" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E244" t="s">
         <v>1</v>
@@ -18128,15 +18182,15 @@
         <v>116</v>
       </c>
       <c r="BD244" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="245" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
+        <v>403</v>
+      </c>
+      <c r="B245" t="s">
         <v>404</v>
-      </c>
-      <c r="B245" t="s">
-        <v>405</v>
       </c>
       <c r="C245" t="s">
         <v>1</v>
@@ -18196,18 +18250,18 @@
         <v>9</v>
       </c>
       <c r="BC245" t="s">
+        <v>405</v>
+      </c>
+      <c r="BD245" t="s">
         <v>406</v>
-      </c>
-      <c r="BD245" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="246" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B246" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C246" t="s">
         <v>1</v>
@@ -18267,18 +18321,18 @@
         <v>9</v>
       </c>
       <c r="BC246" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="BD246" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="247" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B247" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C247" t="s">
         <v>1</v>
@@ -18338,18 +18392,18 @@
         <v>9</v>
       </c>
       <c r="BC247" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="BD247" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="248" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B248" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C248" t="s">
         <v>1</v>
@@ -18409,18 +18463,18 @@
         <v>9</v>
       </c>
       <c r="BC248" t="s">
+        <v>405</v>
+      </c>
+      <c r="BD248" t="s">
         <v>406</v>
-      </c>
-      <c r="BD248" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="249" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B249" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C249" t="s">
         <v>1</v>
@@ -18480,18 +18534,18 @@
         <v>9</v>
       </c>
       <c r="BC249" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="BD249" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="250" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B250" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C250" t="s">
         <v>1</v>
@@ -18551,24 +18605,24 @@
         <v>9</v>
       </c>
       <c r="BC250" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="BD250" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="251" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
+        <v>414</v>
+      </c>
+      <c r="B251" t="s">
+        <v>1</v>
+      </c>
+      <c r="C251" t="s">
+        <v>1</v>
+      </c>
+      <c r="D251" t="s">
         <v>415</v>
-      </c>
-      <c r="B251" t="s">
-        <v>1</v>
-      </c>
-      <c r="C251" t="s">
-        <v>1</v>
-      </c>
-      <c r="D251" t="s">
-        <v>416</v>
       </c>
       <c r="E251" t="s">
         <v>1</v>
@@ -18616,12 +18670,12 @@
         <v>116</v>
       </c>
       <c r="BD251" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="252" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B252" t="s">
         <v>1</v>
@@ -18684,12 +18738,12 @@
         <v>116</v>
       </c>
       <c r="BD252" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="253" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B253" t="s">
         <v>1</v>
@@ -18698,7 +18752,7 @@
         <v>2</v>
       </c>
       <c r="D253" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E253" t="s">
         <v>1</v>
@@ -18752,12 +18806,12 @@
         <v>116</v>
       </c>
       <c r="BD253" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="254" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B254" t="s">
         <v>1</v>
@@ -18766,7 +18820,7 @@
         <v>2</v>
       </c>
       <c r="D254" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E254" t="s">
         <v>1</v>
@@ -18820,12 +18874,12 @@
         <v>116</v>
       </c>
       <c r="BD254" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="255" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B255" t="s">
         <v>1</v>
@@ -18834,7 +18888,7 @@
         <v>2</v>
       </c>
       <c r="D255" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E255" t="s">
         <v>1</v>
@@ -18888,21 +18942,21 @@
         <v>116</v>
       </c>
       <c r="BD255" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="256" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
+        <v>422</v>
+      </c>
+      <c r="B256" t="s">
+        <v>1</v>
+      </c>
+      <c r="C256" t="s">
+        <v>1</v>
+      </c>
+      <c r="D256" t="s">
         <v>423</v>
-      </c>
-      <c r="B256" t="s">
-        <v>1</v>
-      </c>
-      <c r="C256" t="s">
-        <v>1</v>
-      </c>
-      <c r="D256" t="s">
-        <v>424</v>
       </c>
       <c r="E256" t="s">
         <v>1</v>
@@ -18950,12 +19004,12 @@
         <v>116</v>
       </c>
       <c r="BD256" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="257" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B257" t="s">
         <v>1</v>
@@ -19012,21 +19066,21 @@
         <v>116</v>
       </c>
       <c r="BD257" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="258" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
+        <v>425</v>
+      </c>
+      <c r="B258" t="s">
+        <v>1</v>
+      </c>
+      <c r="C258" t="s">
+        <v>1</v>
+      </c>
+      <c r="D258" t="s">
         <v>426</v>
-      </c>
-      <c r="B258" t="s">
-        <v>1</v>
-      </c>
-      <c r="C258" t="s">
-        <v>1</v>
-      </c>
-      <c r="D258" t="s">
-        <v>427</v>
       </c>
       <c r="E258" t="s">
         <v>1</v>
@@ -19074,12 +19128,12 @@
         <v>116</v>
       </c>
       <c r="BD258" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="259" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B259" t="s">
         <v>1</v>
@@ -19088,7 +19142,7 @@
         <v>1</v>
       </c>
       <c r="D259" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E259" t="s">
         <v>1</v>
@@ -19136,12 +19190,12 @@
         <v>116</v>
       </c>
       <c r="BD259" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="260" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B260" t="s">
         <v>1</v>
@@ -19198,7 +19252,7 @@
         <v>116</v>
       </c>
       <c r="BD260" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="261" spans="1:56" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made notes re: aggregation. Made simpler aggregation script.
</commit_message>
<xml_diff>
--- a/edited_data.xlsx
+++ b/edited_data.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhilgard\Documents\GitHub\greietemeyer_meta\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12885"/>
   </bookViews>
@@ -10,9 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AT$369</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AT$370</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3264" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3282" uniqueCount="513">
   <si>
     <t>Adachi, P. J. C., &amp; Willoughby, T. (2011). S1</t>
   </si>
@@ -1546,6 +1551,21 @@
   </si>
   <si>
     <t>d = 0.44</t>
+  </si>
+  <si>
+    <t>Aggressive word completion</t>
+  </si>
+  <si>
+    <t>Aggressive story completion</t>
+  </si>
+  <si>
+    <t>Prosocial word completion</t>
+  </si>
+  <si>
+    <t>prosocial story completion</t>
+  </si>
+  <si>
+    <t>Pooling nonviolent and no-game control in all three studies.</t>
   </si>
 </sst>
 </file>
@@ -1872,7 +1892,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1880,11 +1900,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD368"/>
+  <dimension ref="A1:BD369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK235" sqref="AK235"/>
+      <selection pane="bottomLeft" activeCell="AU237" sqref="AU237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17465,6 +17485,9 @@
       </c>
       <c r="AZ234">
         <v>-1.8762669999999999E-2</v>
+      </c>
+      <c r="BC234" t="s">
+        <v>512</v>
       </c>
       <c r="BD234" t="s">
         <v>389</v>
@@ -17721,63 +17744,86 @@
       <c r="AC237" s="3"/>
       <c r="AD237" s="3"/>
       <c r="AE237" s="3"/>
-      <c r="AF237" s="3"/>
+      <c r="AF237" s="3">
+        <v>111</v>
+      </c>
       <c r="AG237" s="3"/>
       <c r="AH237" s="3"/>
       <c r="AI237" s="3"/>
       <c r="AJ237" s="3"/>
+      <c r="AO237" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP237" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ237" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR237" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU237" t="s">
+        <v>508</v>
+      </c>
+      <c r="AV237" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="238" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>392</v>
-      </c>
-      <c r="B238" t="s">
-        <v>1</v>
-      </c>
-      <c r="C238" t="s">
-        <v>2</v>
-      </c>
-      <c r="D238" t="s">
-        <v>393</v>
-      </c>
-      <c r="E238" t="s">
-        <v>1</v>
-      </c>
-      <c r="F238" t="s">
-        <v>19</v>
-      </c>
-      <c r="J238">
-        <v>0.2</v>
-      </c>
-      <c r="K238">
-        <v>1.3947421999999999E-2</v>
-      </c>
-      <c r="L238">
-        <v>137</v>
-      </c>
-      <c r="M238">
-        <v>152</v>
-      </c>
-      <c r="N238">
-        <v>3</v>
-      </c>
-      <c r="AK238" s="1">
-        <v>9.9370925693902504E-2</v>
-      </c>
-      <c r="AL238" s="1">
-        <v>5.80987141556355E-2</v>
-      </c>
-      <c r="AM238">
-        <v>9.9699959427935997E-2</v>
-      </c>
-      <c r="AN238" s="1">
-        <v>5.8678136156606199E-2</v>
-      </c>
+      <c r="A238" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F238" s="3"/>
+      <c r="G238" s="3"/>
+      <c r="H238" s="3"/>
+      <c r="I238" s="3"/>
+      <c r="J238" s="3"/>
+      <c r="K238" s="3"/>
+      <c r="L238" s="3"/>
+      <c r="M238" s="3"/>
+      <c r="N238" s="3"/>
+      <c r="O238" s="3"/>
+      <c r="P238" s="3"/>
+      <c r="Q238" s="3"/>
+      <c r="R238" s="3"/>
+      <c r="S238" s="3"/>
+      <c r="T238" s="3"/>
+      <c r="U238" s="3"/>
+      <c r="V238" s="3"/>
+      <c r="W238" s="3"/>
+      <c r="X238" s="3"/>
+      <c r="Y238" s="3"/>
+      <c r="Z238" s="3"/>
+      <c r="AA238" s="3"/>
+      <c r="AB238" s="3"/>
+      <c r="AC238" s="3"/>
+      <c r="AD238" s="3"/>
+      <c r="AE238" s="3"/>
+      <c r="AF238" s="3">
+        <v>111</v>
+      </c>
+      <c r="AG238" s="3"/>
+      <c r="AH238" s="3"/>
+      <c r="AI238" s="3"/>
+      <c r="AJ238" s="3"/>
       <c r="AO238" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="AP238" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="AQ238" t="s">
         <v>7</v>
@@ -17785,19 +17831,16 @@
       <c r="AR238" t="s">
         <v>8</v>
       </c>
-      <c r="AS238">
-        <v>3</v>
-      </c>
-      <c r="AT238" t="s">
-        <v>116</v>
-      </c>
-      <c r="BD238" t="s">
-        <v>394</v>
+      <c r="AU238" t="s">
+        <v>510</v>
+      </c>
+      <c r="AV238" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="239" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B239" t="s">
         <v>1</v>
@@ -17806,7 +17849,7 @@
         <v>2</v>
       </c>
       <c r="D239" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E239" t="s">
         <v>1</v>
@@ -17815,34 +17858,34 @@
         <v>19</v>
       </c>
       <c r="J239">
-        <v>0.37</v>
+        <v>0.2</v>
       </c>
       <c r="K239">
-        <v>3.0884330000000002E-2</v>
+        <v>1.3947421999999999E-2</v>
       </c>
       <c r="L239">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="M239">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="N239">
-        <v>1</v>
-      </c>
-      <c r="AK239">
-        <v>0.181731388425629</v>
+        <v>3</v>
+      </c>
+      <c r="AK239" s="1">
+        <v>9.9370925693902504E-2</v>
       </c>
       <c r="AL239" s="1">
-        <v>8.3466456439473397E-2</v>
+        <v>5.80987141556355E-2</v>
       </c>
       <c r="AM239">
-        <v>0.183772630839275</v>
+        <v>9.9699959427935997E-2</v>
       </c>
       <c r="AN239" s="1">
-        <v>8.6317193763445696E-2</v>
+        <v>5.8678136156606199E-2</v>
       </c>
       <c r="AO239" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="AP239" t="s">
         <v>6</v>
@@ -17860,7 +17903,7 @@
         <v>116</v>
       </c>
       <c r="BD239" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="240" spans="1:56" x14ac:dyDescent="0.25">
@@ -17874,7 +17917,7 @@
         <v>2</v>
       </c>
       <c r="D240" t="s">
-        <v>245</v>
+        <v>396</v>
       </c>
       <c r="E240" t="s">
         <v>1</v>
@@ -17883,10 +17926,10 @@
         <v>19</v>
       </c>
       <c r="J240">
-        <v>-0.05</v>
+        <v>0.37</v>
       </c>
       <c r="K240">
-        <v>3.0375238999999998E-2</v>
+        <v>3.0884330000000002E-2</v>
       </c>
       <c r="L240">
         <v>63</v>
@@ -17895,25 +17938,25 @@
         <v>69</v>
       </c>
       <c r="N240">
-        <v>3</v>
-      </c>
-      <c r="AK240" s="1">
-        <v>2.49663755409265E-2</v>
+        <v>1</v>
+      </c>
+      <c r="AK240">
+        <v>0.181731388425629</v>
       </c>
       <c r="AL240" s="1">
-        <v>8.6971018806489594E-2</v>
-      </c>
-      <c r="AM240" s="1">
-        <v>2.49715648281152E-2</v>
+        <v>8.3466456439473397E-2</v>
+      </c>
+      <c r="AM240">
+        <v>0.183772630839275</v>
       </c>
       <c r="AN240" s="1">
-        <v>8.7025263385626397E-2</v>
+        <v>8.6317193763445696E-2</v>
       </c>
       <c r="AO240" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="AP240" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="AQ240" t="s">
         <v>7</v>
@@ -17942,7 +17985,7 @@
         <v>2</v>
       </c>
       <c r="D241" t="s">
-        <v>398</v>
+        <v>245</v>
       </c>
       <c r="E241" t="s">
         <v>1</v>
@@ -17951,10 +17994,10 @@
         <v>19</v>
       </c>
       <c r="J241">
-        <v>0.37</v>
+        <v>-0.05</v>
       </c>
       <c r="K241">
-        <v>3.0884330000000002E-2</v>
+        <v>3.0375238999999998E-2</v>
       </c>
       <c r="L241">
         <v>63</v>
@@ -17963,25 +18006,25 @@
         <v>69</v>
       </c>
       <c r="N241">
-        <v>1</v>
-      </c>
-      <c r="AK241">
-        <v>0.181731388425629</v>
+        <v>3</v>
+      </c>
+      <c r="AK241" s="1">
+        <v>2.49663755409265E-2</v>
       </c>
       <c r="AL241" s="1">
-        <v>8.3466456439473397E-2</v>
-      </c>
-      <c r="AM241">
-        <v>0.183772630839275</v>
+        <v>8.6971018806489594E-2</v>
+      </c>
+      <c r="AM241" s="1">
+        <v>2.49715648281152E-2</v>
       </c>
       <c r="AN241" s="1">
-        <v>8.6317193763445696E-2</v>
+        <v>8.7025263385626397E-2</v>
       </c>
       <c r="AO241" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="AP241" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="AQ241" t="s">
         <v>7</v>
@@ -18001,52 +18044,58 @@
     </row>
     <row r="242" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B242" t="s">
         <v>1</v>
       </c>
       <c r="C242" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D242" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E242" t="s">
         <v>1</v>
       </c>
       <c r="F242" t="s">
-        <v>4</v>
-      </c>
-      <c r="G242">
-        <v>0.19</v>
-      </c>
-      <c r="H242">
-        <v>168</v>
-      </c>
-      <c r="I242">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="J242">
+        <v>0.37</v>
+      </c>
+      <c r="K242">
+        <v>3.0884330000000002E-2</v>
+      </c>
+      <c r="L242">
+        <v>63</v>
+      </c>
+      <c r="M242">
+        <v>69</v>
+      </c>
+      <c r="N242">
+        <v>1</v>
       </c>
       <c r="AK242">
-        <v>0.19</v>
+        <v>0.181731388425629</v>
       </c>
       <c r="AL242" s="1">
-        <v>7.5039513227729199E-2</v>
-      </c>
-      <c r="AM242" s="1">
-        <v>0.192337169219545</v>
+        <v>8.3466456439473397E-2</v>
+      </c>
+      <c r="AM242">
+        <v>0.183772630839275</v>
       </c>
       <c r="AN242" s="1">
-        <v>7.7849894416152296E-2</v>
+        <v>8.6317193763445696E-2</v>
       </c>
       <c r="AO242" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="AP242" t="s">
         <v>6</v>
       </c>
       <c r="AQ242" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="AR242" t="s">
         <v>8</v>
@@ -18058,7 +18107,7 @@
         <v>116</v>
       </c>
       <c r="BD242" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="243" spans="1:56" x14ac:dyDescent="0.25">
@@ -18072,7 +18121,7 @@
         <v>1</v>
       </c>
       <c r="D243" t="s">
-        <v>293</v>
+        <v>400</v>
       </c>
       <c r="E243" t="s">
         <v>1</v>
@@ -18081,7 +18130,7 @@
         <v>4</v>
       </c>
       <c r="G243">
-        <v>0.28999999999999998</v>
+        <v>0.19</v>
       </c>
       <c r="H243">
         <v>168</v>
@@ -18090,19 +18139,19 @@
         <v>3</v>
       </c>
       <c r="AK243">
-        <v>0.28999999999999998</v>
+        <v>0.19</v>
       </c>
       <c r="AL243" s="1">
-        <v>7.1302718295753895E-2</v>
+        <v>7.5039513227729199E-2</v>
       </c>
       <c r="AM243" s="1">
-        <v>0.29856626366017802</v>
+        <v>0.192337169219545</v>
       </c>
       <c r="AN243" s="1">
         <v>7.7849894416152296E-2</v>
       </c>
       <c r="AO243" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="AP243" t="s">
         <v>6</v>
@@ -18134,7 +18183,7 @@
         <v>1</v>
       </c>
       <c r="D244" t="s">
-        <v>402</v>
+        <v>293</v>
       </c>
       <c r="E244" t="s">
         <v>1</v>
@@ -18143,7 +18192,7 @@
         <v>4</v>
       </c>
       <c r="G244">
-        <v>0.23</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H244">
         <v>168</v>
@@ -18152,19 +18201,19 @@
         <v>3</v>
       </c>
       <c r="AK244">
-        <v>0.23</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="AL244" s="1">
-        <v>7.3731635001537801E-2</v>
-      </c>
-      <c r="AM244">
-        <v>0.234189466759367</v>
+        <v>7.1302718295753895E-2</v>
+      </c>
+      <c r="AM244" s="1">
+        <v>0.29856626366017802</v>
       </c>
       <c r="AN244" s="1">
         <v>7.7849894416152296E-2</v>
       </c>
       <c r="AO244" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="AP244" t="s">
         <v>6</v>
@@ -18187,49 +18236,43 @@
     </row>
     <row r="245" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B245" t="s">
-        <v>404</v>
+        <v>1</v>
       </c>
       <c r="C245" t="s">
         <v>1</v>
       </c>
       <c r="D245" t="s">
-        <v>44</v>
+        <v>402</v>
       </c>
       <c r="E245" t="s">
         <v>1</v>
       </c>
       <c r="F245" t="s">
-        <v>19</v>
-      </c>
-      <c r="J245">
-        <v>0.521058574</v>
-      </c>
-      <c r="K245">
-        <v>0.15946897700000001</v>
-      </c>
-      <c r="L245">
-        <v>14</v>
-      </c>
-      <c r="M245">
-        <v>14</v>
-      </c>
-      <c r="N245">
+        <v>4</v>
+      </c>
+      <c r="G245">
+        <v>0.23</v>
+      </c>
+      <c r="H245">
+        <v>168</v>
+      </c>
+      <c r="I245">
         <v>3</v>
       </c>
       <c r="AK245">
-        <v>0.252113578984761</v>
-      </c>
-      <c r="AL245">
-        <v>0.18093690974440399</v>
+        <v>0.23</v>
+      </c>
+      <c r="AL245" s="1">
+        <v>7.3731635001537801E-2</v>
       </c>
       <c r="AM245">
-        <v>0.25766857135089799</v>
-      </c>
-      <c r="AN245">
-        <v>0.193218094659804</v>
+        <v>0.234189466759367</v>
+      </c>
+      <c r="AN245" s="1">
+        <v>7.7849894416152296E-2</v>
       </c>
       <c r="AO245" t="s">
         <v>26</v>
@@ -18238,22 +18281,19 @@
         <v>6</v>
       </c>
       <c r="AQ245" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="AR245" t="s">
         <v>8</v>
       </c>
       <c r="AS245">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AT245" t="s">
-        <v>9</v>
-      </c>
-      <c r="BC245" t="s">
-        <v>405</v>
+        <v>116</v>
       </c>
       <c r="BD245" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="246" spans="1:56" x14ac:dyDescent="0.25">
@@ -18261,7 +18301,7 @@
         <v>403</v>
       </c>
       <c r="B246" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C246" t="s">
         <v>1</v>
@@ -18275,11 +18315,11 @@
       <c r="F246" t="s">
         <v>19</v>
       </c>
-      <c r="J246" s="2">
-        <v>1.3160066509999999</v>
+      <c r="J246">
+        <v>0.521058574</v>
       </c>
       <c r="K246">
-        <v>0.189713357</v>
+        <v>0.15946897700000001</v>
       </c>
       <c r="L246">
         <v>14</v>
@@ -18291,16 +18331,16 @@
         <v>3</v>
       </c>
       <c r="AK246">
-        <v>0.54967980997843602</v>
+        <v>0.252113578984761</v>
       </c>
       <c r="AL246">
-        <v>0.126959162679183</v>
+        <v>0.18093690974440399</v>
       </c>
       <c r="AM246">
-        <v>0.61792237562034202</v>
+        <v>0.25766857135089799</v>
       </c>
       <c r="AN246">
-        <v>0.18192846520956299</v>
+        <v>0.193218094659804</v>
       </c>
       <c r="AO246" t="s">
         <v>26</v>
@@ -18321,7 +18361,7 @@
         <v>9</v>
       </c>
       <c r="BC246" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="BD246" t="s">
         <v>406</v>
@@ -18332,7 +18372,7 @@
         <v>403</v>
       </c>
       <c r="B247" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C247" t="s">
         <v>1</v>
@@ -18346,32 +18386,32 @@
       <c r="F247" t="s">
         <v>19</v>
       </c>
-      <c r="J247">
-        <v>0.24728792099999999</v>
+      <c r="J247" s="2">
+        <v>1.3160066509999999</v>
       </c>
       <c r="K247">
-        <v>0.11859924199999999</v>
+        <v>0.189713357</v>
       </c>
       <c r="L247">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M247">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="N247">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK247">
-        <v>-0.122709537072517</v>
+        <v>0.54967980997843602</v>
       </c>
       <c r="AL247">
-        <v>0.168316693485384</v>
+        <v>0.126959162679183</v>
       </c>
       <c r="AM247">
-        <v>-0.12333106702734301</v>
+        <v>0.61792237562034202</v>
       </c>
       <c r="AN247">
-        <v>0.170889890307869</v>
+        <v>0.18192846520956299</v>
       </c>
       <c r="AO247" t="s">
         <v>26</v>
@@ -18392,7 +18432,7 @@
         <v>9</v>
       </c>
       <c r="BC247" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="BD247" t="s">
         <v>406</v>
@@ -18403,7 +18443,7 @@
         <v>403</v>
       </c>
       <c r="B248" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C248" t="s">
         <v>1</v>
@@ -18418,31 +18458,31 @@
         <v>19</v>
       </c>
       <c r="J248">
-        <v>0.44937575200000002</v>
+        <v>0.24728792099999999</v>
       </c>
       <c r="K248">
-        <v>0.10265044399999999</v>
+        <v>0.11859924199999999</v>
       </c>
       <c r="L248">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M248">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N248">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK248">
-        <v>0.21922232790873999</v>
+        <v>-0.122709537072517</v>
       </c>
       <c r="AL248">
-        <v>0.14878729886288</v>
+        <v>0.168316693485384</v>
       </c>
       <c r="AM248">
-        <v>0.22283902992136101</v>
+        <v>-0.12333106702734301</v>
       </c>
       <c r="AN248">
-        <v>0.156298772323787</v>
+        <v>0.170889890307869</v>
       </c>
       <c r="AO248" t="s">
         <v>26</v>
@@ -18463,7 +18503,7 @@
         <v>9</v>
       </c>
       <c r="BC248" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="BD248" t="s">
         <v>406</v>
@@ -18474,7 +18514,7 @@
         <v>403</v>
       </c>
       <c r="B249" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C249" t="s">
         <v>1</v>
@@ -18489,31 +18529,31 @@
         <v>19</v>
       </c>
       <c r="J249">
-        <v>0.627600096</v>
+        <v>0.44937575200000002</v>
       </c>
       <c r="K249">
-        <v>0.123780168</v>
+        <v>0.10265044399999999</v>
       </c>
       <c r="L249">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M249">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="N249">
         <v>3</v>
       </c>
       <c r="AK249">
-        <v>0.29940483715614602</v>
+        <v>0.21922232790873999</v>
       </c>
       <c r="AL249">
-        <v>0.15279634250882601</v>
+        <v>0.14878729886288</v>
       </c>
       <c r="AM249">
-        <v>0.30886570730625501</v>
+        <v>0.22283902992136101</v>
       </c>
       <c r="AN249">
-        <v>0.16784227018902001</v>
+        <v>0.156298772323787</v>
       </c>
       <c r="AO249" t="s">
         <v>26</v>
@@ -18534,7 +18574,7 @@
         <v>9</v>
       </c>
       <c r="BC249" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="BD249" t="s">
         <v>406</v>
@@ -18545,7 +18585,7 @@
         <v>403</v>
       </c>
       <c r="B250" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C250" t="s">
         <v>1</v>
@@ -18560,31 +18600,31 @@
         <v>19</v>
       </c>
       <c r="J250">
-        <v>0.36363537600000001</v>
+        <v>0.627600096</v>
       </c>
       <c r="K250">
-        <v>0.14538706700000001</v>
+        <v>0.123780168</v>
       </c>
       <c r="L250">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M250">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="N250">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK250">
-        <v>-0.17888496789436301</v>
+        <v>0.29940483715614602</v>
       </c>
       <c r="AL250">
-        <v>0.18157081425836399</v>
+        <v>0.15279634250882601</v>
       </c>
       <c r="AM250">
-        <v>-0.18083055821648</v>
+        <v>0.30886570730625501</v>
       </c>
       <c r="AN250">
-        <v>0.18757312262091</v>
+        <v>0.16784227018902001</v>
       </c>
       <c r="AO250" t="s">
         <v>26</v>
@@ -18605,7 +18645,7 @@
         <v>9</v>
       </c>
       <c r="BC250" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="BD250" t="s">
         <v>406</v>
@@ -18613,111 +18653,114 @@
     </row>
     <row r="251" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="B251" t="s">
-        <v>1</v>
+        <v>413</v>
       </c>
       <c r="C251" t="s">
         <v>1</v>
       </c>
       <c r="D251" t="s">
-        <v>415</v>
+        <v>44</v>
       </c>
       <c r="E251" t="s">
         <v>1</v>
       </c>
       <c r="F251" t="s">
-        <v>4</v>
-      </c>
-      <c r="G251">
-        <v>0.24</v>
-      </c>
-      <c r="H251">
-        <v>234</v>
-      </c>
-      <c r="I251">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="J251">
+        <v>0.36363537600000001</v>
+      </c>
+      <c r="K251">
+        <v>0.14538706700000001</v>
+      </c>
+      <c r="L251">
+        <v>15</v>
+      </c>
+      <c r="M251">
+        <v>15</v>
+      </c>
+      <c r="N251">
+        <v>2</v>
       </c>
       <c r="AK251">
-        <v>0.24</v>
-      </c>
-      <c r="AL251" s="1">
-        <v>6.2005367733008597E-2</v>
+        <v>-0.17888496789436301</v>
+      </c>
+      <c r="AL251">
+        <v>0.18157081425836399</v>
       </c>
       <c r="AM251">
-        <v>0.244774112659353</v>
-      </c>
-      <c r="AN251" s="1">
-        <v>6.5795169495976899E-2</v>
+        <v>-0.18083055821648</v>
+      </c>
+      <c r="AN251">
+        <v>0.18757312262091</v>
       </c>
       <c r="AO251" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="AP251" t="s">
         <v>6</v>
       </c>
       <c r="AQ251" t="s">
-        <v>115</v>
+        <v>7</v>
       </c>
       <c r="AR251" t="s">
         <v>8</v>
       </c>
       <c r="AS251">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AT251" t="s">
-        <v>116</v>
+        <v>9</v>
+      </c>
+      <c r="BC251" t="s">
+        <v>410</v>
       </c>
       <c r="BD251" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
     </row>
     <row r="252" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B252" t="s">
         <v>1</v>
       </c>
       <c r="C252" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D252" t="s">
-        <v>263</v>
+        <v>415</v>
       </c>
       <c r="E252" t="s">
         <v>1</v>
       </c>
       <c r="F252" t="s">
-        <v>19</v>
-      </c>
-      <c r="J252">
-        <v>0.44</v>
-      </c>
-      <c r="K252">
-        <v>2.7311999999999999E-2</v>
-      </c>
-      <c r="L252">
-        <v>75</v>
-      </c>
-      <c r="M252">
-        <v>75</v>
-      </c>
-      <c r="N252">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="G252">
+        <v>0.24</v>
+      </c>
+      <c r="H252">
+        <v>234</v>
+      </c>
+      <c r="I252">
+        <v>3</v>
       </c>
       <c r="AK252">
-        <v>0.21486178267511999</v>
-      </c>
-      <c r="AL252">
-        <v>7.6976159209578995E-2</v>
+        <v>0.24</v>
+      </c>
+      <c r="AL252" s="1">
+        <v>6.2005367733008597E-2</v>
       </c>
       <c r="AM252">
-        <v>0.218262907439882</v>
+        <v>0.244774112659353</v>
       </c>
       <c r="AN252" s="1">
-        <v>8.0701805315322603E-2</v>
+        <v>6.5795169495976899E-2</v>
       </c>
       <c r="AO252" t="s">
         <v>5</v>
@@ -18726,19 +18769,19 @@
         <v>6</v>
       </c>
       <c r="AQ252" t="s">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="AR252" t="s">
         <v>8</v>
       </c>
       <c r="AS252">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AT252" t="s">
         <v>116</v>
       </c>
       <c r="BD252" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="253" spans="1:56" x14ac:dyDescent="0.25">
@@ -18752,7 +18795,7 @@
         <v>2</v>
       </c>
       <c r="D253" t="s">
-        <v>419</v>
+        <v>263</v>
       </c>
       <c r="E253" t="s">
         <v>1</v>
@@ -18761,10 +18804,10 @@
         <v>19</v>
       </c>
       <c r="J253">
-        <v>-0.39</v>
+        <v>0.44</v>
       </c>
       <c r="K253">
-        <v>2.7173666999999999E-2</v>
+        <v>2.7311999999999999E-2</v>
       </c>
       <c r="L253">
         <v>75</v>
@@ -18773,25 +18816,25 @@
         <v>75</v>
       </c>
       <c r="N253">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK253">
-        <v>0.191395051403356</v>
-      </c>
-      <c r="AL253" s="1">
-        <v>7.7934976527938807E-2</v>
+        <v>0.21486178267511999</v>
+      </c>
+      <c r="AL253">
+        <v>7.6976159209578995E-2</v>
       </c>
       <c r="AM253">
-        <v>0.19378486722187599</v>
+        <v>0.218262907439882</v>
       </c>
       <c r="AN253" s="1">
-        <v>8.0898454010413706E-2</v>
+        <v>8.0701805315322603E-2</v>
       </c>
       <c r="AO253" t="s">
         <v>5</v>
       </c>
       <c r="AP253" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="AQ253" t="s">
         <v>7</v>
@@ -18820,7 +18863,7 @@
         <v>2</v>
       </c>
       <c r="D254" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E254" t="s">
         <v>1</v>
@@ -18829,31 +18872,31 @@
         <v>19</v>
       </c>
       <c r="J254">
-        <v>7.0000000000000007E-2</v>
+        <v>-0.39</v>
       </c>
       <c r="K254">
-        <v>3.4503879000000001E-2</v>
+        <v>2.7173666999999999E-2</v>
       </c>
       <c r="L254">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="M254">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="N254">
-        <v>1</v>
-      </c>
-      <c r="AK254" s="1">
-        <v>3.4978582175618597E-2</v>
+        <v>3</v>
+      </c>
+      <c r="AK254">
+        <v>0.191395051403356</v>
       </c>
       <c r="AL254" s="1">
-        <v>9.2705700034930505E-2</v>
-      </c>
-      <c r="AM254" s="1">
-        <v>3.4992858102937403E-2</v>
+        <v>7.7934976527938807E-2</v>
+      </c>
+      <c r="AM254">
+        <v>0.19378486722187599</v>
       </c>
       <c r="AN254" s="1">
-        <v>9.2819264517473299E-2</v>
+        <v>8.0898454010413706E-2</v>
       </c>
       <c r="AO254" t="s">
         <v>5</v>
@@ -18888,7 +18931,7 @@
         <v>2</v>
       </c>
       <c r="D255" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E255" t="s">
         <v>1</v>
@@ -18897,31 +18940,31 @@
         <v>19</v>
       </c>
       <c r="J255">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K255">
-        <v>2.6700000000000002E-2</v>
+        <v>3.4503879000000001E-2</v>
       </c>
       <c r="L255">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="M255">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="N255">
         <v>1</v>
       </c>
       <c r="AK255" s="1">
-        <v>4.9937616943892198E-2</v>
+        <v>3.4978582175618597E-2</v>
       </c>
       <c r="AL255" s="1">
-        <v>8.1395250312464404E-2</v>
+        <v>9.2705700034930505E-2</v>
       </c>
       <c r="AM255" s="1">
-        <v>4.99791900693487E-2</v>
+        <v>3.4992858102937403E-2</v>
       </c>
       <c r="AN255" s="1">
-        <v>8.1598738438245597E-2</v>
+        <v>9.2819264517473299E-2</v>
       </c>
       <c r="AO255" t="s">
         <v>5</v>
@@ -18947,69 +18990,75 @@
     </row>
     <row r="256" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B256" t="s">
         <v>1</v>
       </c>
       <c r="C256" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D256" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E256" t="s">
         <v>1</v>
       </c>
       <c r="F256" t="s">
-        <v>4</v>
-      </c>
-      <c r="G256">
-        <v>0.24</v>
-      </c>
-      <c r="H256">
-        <v>1492</v>
-      </c>
-      <c r="I256">
-        <v>3</v>
-      </c>
-      <c r="AK256">
-        <v>0.24</v>
+        <v>19</v>
+      </c>
+      <c r="J256">
+        <v>0.1</v>
+      </c>
+      <c r="K256">
+        <v>2.6700000000000002E-2</v>
+      </c>
+      <c r="L256">
+        <v>75</v>
+      </c>
+      <c r="M256">
+        <v>75</v>
+      </c>
+      <c r="N256">
+        <v>1</v>
+      </c>
+      <c r="AK256" s="1">
+        <v>4.9937616943892198E-2</v>
       </c>
       <c r="AL256" s="1">
-        <v>2.44223768623184E-2</v>
-      </c>
-      <c r="AM256">
-        <v>0.244774112659353</v>
+        <v>8.1395250312464404E-2</v>
+      </c>
+      <c r="AM256" s="1">
+        <v>4.99791900693487E-2</v>
       </c>
       <c r="AN256" s="1">
-        <v>2.5915085804667198E-2</v>
+        <v>8.1598738438245597E-2</v>
       </c>
       <c r="AO256" t="s">
         <v>5</v>
       </c>
       <c r="AP256" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="AQ256" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="AR256" t="s">
         <v>8</v>
       </c>
       <c r="AS256">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT256" t="s">
         <v>116</v>
       </c>
       <c r="BD256" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="257" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B257" t="s">
         <v>1</v>
@@ -19018,7 +19067,7 @@
         <v>1</v>
       </c>
       <c r="D257" t="s">
-        <v>245</v>
+        <v>423</v>
       </c>
       <c r="E257" t="s">
         <v>1</v>
@@ -19027,28 +19076,28 @@
         <v>4</v>
       </c>
       <c r="G257">
-        <v>0.28000000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="H257">
-        <v>795</v>
+        <v>1492</v>
       </c>
       <c r="I257">
         <v>3</v>
       </c>
       <c r="AK257">
-        <v>0.28000000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="AL257" s="1">
-        <v>3.2747630032221801E-2</v>
+        <v>2.44223768623184E-2</v>
       </c>
       <c r="AM257">
-        <v>0.28768207245178101</v>
+        <v>0.244774112659353</v>
       </c>
       <c r="AN257" s="1">
-        <v>3.5533452725935097E-2</v>
+        <v>2.5915085804667198E-2</v>
       </c>
       <c r="AO257" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AP257" t="s">
         <v>6</v>
@@ -19066,7 +19115,7 @@
         <v>116</v>
       </c>
       <c r="BD257" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="258" spans="1:56" x14ac:dyDescent="0.25">
@@ -19080,7 +19129,7 @@
         <v>1</v>
       </c>
       <c r="D258" t="s">
-        <v>426</v>
+        <v>245</v>
       </c>
       <c r="E258" t="s">
         <v>1</v>
@@ -19089,7 +19138,7 @@
         <v>4</v>
       </c>
       <c r="G258">
-        <v>-0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H258">
         <v>795</v>
@@ -19098,13 +19147,13 @@
         <v>3</v>
       </c>
       <c r="AK258">
-        <v>0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AL258" s="1">
-        <v>3.3813633613999798E-2</v>
+        <v>3.2747630032221801E-2</v>
       </c>
       <c r="AM258">
-        <v>0.223656109021832</v>
+        <v>0.28768207245178101</v>
       </c>
       <c r="AN258" s="1">
         <v>3.5533452725935097E-2</v>
@@ -19142,7 +19191,7 @@
         <v>1</v>
       </c>
       <c r="D259" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E259" t="s">
         <v>1</v>
@@ -19151,7 +19200,7 @@
         <v>4</v>
       </c>
       <c r="G259">
-        <v>0.19</v>
+        <v>-0.22</v>
       </c>
       <c r="H259">
         <v>795</v>
@@ -19160,13 +19209,13 @@
         <v>3</v>
       </c>
       <c r="AK259">
-        <v>0.19</v>
+        <v>0.22</v>
       </c>
       <c r="AL259" s="1">
-        <v>3.4250695082528801E-2</v>
+        <v>3.3813633613999798E-2</v>
       </c>
       <c r="AM259">
-        <v>0.192337169219545</v>
+        <v>0.223656109021832</v>
       </c>
       <c r="AN259" s="1">
         <v>3.5533452725935097E-2</v>
@@ -19204,7 +19253,7 @@
         <v>1</v>
       </c>
       <c r="D260" t="s">
-        <v>293</v>
+        <v>428</v>
       </c>
       <c r="E260" t="s">
         <v>1</v>
@@ -19213,7 +19262,7 @@
         <v>4</v>
       </c>
       <c r="G260">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="H260">
         <v>795</v>
@@ -19222,19 +19271,19 @@
         <v>3</v>
       </c>
       <c r="AK260">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="AL260" s="1">
-        <v>3.5178118198675702E-2</v>
-      </c>
-      <c r="AM260" s="1">
-        <v>0.100335347731076</v>
+        <v>3.4250695082528801E-2</v>
+      </c>
+      <c r="AM260">
+        <v>0.192337169219545</v>
       </c>
       <c r="AN260" s="1">
         <v>3.5533452725935097E-2</v>
       </c>
       <c r="AO260" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AP260" t="s">
         <v>6</v>
@@ -19256,7 +19305,66 @@
       </c>
     </row>
     <row r="261" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="AN261" s="1"/>
+      <c r="A261" t="s">
+        <v>425</v>
+      </c>
+      <c r="B261" t="s">
+        <v>1</v>
+      </c>
+      <c r="C261" t="s">
+        <v>1</v>
+      </c>
+      <c r="D261" t="s">
+        <v>293</v>
+      </c>
+      <c r="E261" t="s">
+        <v>1</v>
+      </c>
+      <c r="F261" t="s">
+        <v>4</v>
+      </c>
+      <c r="G261">
+        <v>0.1</v>
+      </c>
+      <c r="H261">
+        <v>795</v>
+      </c>
+      <c r="I261">
+        <v>3</v>
+      </c>
+      <c r="AK261">
+        <v>0.1</v>
+      </c>
+      <c r="AL261" s="1">
+        <v>3.5178118198675702E-2</v>
+      </c>
+      <c r="AM261" s="1">
+        <v>0.100335347731076</v>
+      </c>
+      <c r="AN261" s="1">
+        <v>3.5533452725935097E-2</v>
+      </c>
+      <c r="AO261" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP261" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ261" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR261" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS261">
+        <v>3</v>
+      </c>
+      <c r="AT261" t="s">
+        <v>116</v>
+      </c>
+      <c r="BD261" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="262" spans="1:56" x14ac:dyDescent="0.25">
       <c r="AN262" s="1"/>
@@ -19279,8 +19387,8 @@
     <row r="268" spans="1:56" x14ac:dyDescent="0.25">
       <c r="AN268" s="1"/>
     </row>
-    <row r="271" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="AN271" s="1"/>
+    <row r="269" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AN269" s="1"/>
     </row>
     <row r="272" spans="1:56" x14ac:dyDescent="0.25">
       <c r="AN272" s="1"/>
@@ -19390,8 +19498,8 @@
     <row r="307" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN307" s="1"/>
     </row>
-    <row r="311" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN311" s="1"/>
+    <row r="308" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN308" s="1"/>
     </row>
     <row r="312" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN312" s="1"/>
@@ -19399,11 +19507,11 @@
     <row r="313" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN313" s="1"/>
     </row>
-    <row r="342" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN342" s="1"/>
-    </row>
-    <row r="365" spans="40:40" x14ac:dyDescent="0.25">
-      <c r="AN365" s="1"/>
+    <row r="314" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN314" s="1"/>
+    </row>
+    <row r="343" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN343" s="1"/>
     </row>
     <row r="366" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN366" s="1"/>
@@ -19414,8 +19522,11 @@
     <row r="368" spans="40:40" x14ac:dyDescent="0.25">
       <c r="AN368" s="1"/>
     </row>
+    <row r="369" spans="40:40" x14ac:dyDescent="0.25">
+      <c r="AN369" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AT369">
+  <autoFilter ref="A1:AT370">
     <sortState ref="A2:AV391">
       <sortCondition ref="A1:A391"/>
     </sortState>

</xml_diff>